<commit_message>
feat: Update Dockerfiles (WIP) + Update readmes (WIP) + Update scripts + Update config example
</commit_message>
<xml_diff>
--- a/examples/common/config.xlsx
+++ b/examples/common/config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Help" sheetId="1" state="visible" r:id="rId2"/>
@@ -154,6 +154,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Optional</t>
     </r>
@@ -163,8 +164,25 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> </t>
+      <t xml:space="preserve"> The list of band names to consider. Separate with `,`.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">integrations</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Optional</t>
     </r>
     <r>
       <rPr>
@@ -174,41 +192,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">The list of band names to consider. Separate with `,`.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">integrations</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Optional</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">The list of integration names to consider. Separate with `,`.</t>
+      <t xml:space="preserve"> The list of integration names to consider. Separate with `,`.</t>
     </r>
   </si>
   <si>
@@ -358,7 +342,7 @@
     <t xml:space="preserve">base_path</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/bamdad/git/sound-scape-explorer/sample-lana</t>
+    <t xml:space="preserve">./project</t>
   </si>
   <si>
     <t xml:space="preserve">The relative or absolute path to your project folder. Examples: “./relative/project” “/absolute/project”.</t>
@@ -462,7 +446,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -518,26 +502,13 @@
       <b val="true"/>
       <i val="true"/>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <i val="true"/>
-      <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -558,32 +529,26 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFA6"/>
+        <bgColor rgb="FFFFFFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFD7"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFEEEEEE"/>
-        <bgColor rgb="FFF6F9D4"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF443205"/>
         <bgColor rgb="FF333333"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFA6"/>
-        <bgColor rgb="FFFFFFD7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF6F9D4"/>
-        <bgColor rgb="FFFFFFD7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFD7"/>
-        <bgColor rgb="FFF6F9D4"/>
       </patternFill>
     </fill>
   </fills>
@@ -628,7 +593,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -642,98 +607,94 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -782,7 +743,7 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFF6F9D4"/>
+      <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFFA6"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
@@ -817,10 +778,10 @@
   </sheetPr>
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="I26" activeCellId="0" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -857,34 +818,34 @@
       <c r="B5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="6" t="s">
         <v>12</v>
       </c>
     </row>
@@ -895,26 +856,26 @@
       <c r="B11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="6" t="s">
         <v>19</v>
       </c>
     </row>
@@ -925,18 +886,18 @@
       <c r="B16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="6" t="s">
         <v>24</v>
       </c>
     </row>
@@ -947,26 +908,26 @@
       <c r="B20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="6" t="s">
         <v>31</v>
       </c>
     </row>
@@ -977,39 +938,39 @@
       <c r="B25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="6" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="8" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="8" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="7" t="s">
         <v>41</v>
       </c>
       <c r="B30" s="8" t="s">
@@ -1023,10 +984,10 @@
       <c r="B32" s="2"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="6" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1037,14 +998,17 @@
       <c r="B35" s="2"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="6" t="s">
         <v>48</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1073,11 +1037,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="24" width="14.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="24" width="17.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="24" width="15.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="24" width="25.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="23" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="23" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="23" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="23" width="25.98"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="6" style="1" width="11.52"/>
   </cols>
   <sheetData>
@@ -1088,31 +1052,31 @@
       <c r="B1" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="24" t="s">
         <v>41</v>
       </c>
       <c r="F1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="22" t="s">
         <v>49</v>
       </c>
       <c r="B2" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="25" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1155,7 +1119,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="13.17"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
@@ -1165,7 +1129,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="22" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1208,7 +1172,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="15.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="15.63"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
@@ -1218,7 +1182,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="22" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1376,7 +1340,7 @@
       <c r="A7" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="6" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1384,7 +1348,7 @@
       <c r="A8" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="6" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1392,7 +1356,7 @@
       <c r="A9" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="6" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1400,7 +1364,7 @@
       <c r="A10" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="6" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1482,16 +1446,16 @@
       <c r="B6" s="12"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="5"/>
+      <c r="B7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="5"/>
+      <c r="B8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="5"/>
+      <c r="B9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="5"/>
+      <c r="B10" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1512,12 +1476,12 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1546,7 +1510,7 @@
       <c r="B2" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1557,7 +1521,7 @@
       <c r="B3" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="6" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1568,7 +1532,7 @@
       <c r="B4" s="15" t="n">
         <v>44100</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="6" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1616,7 +1580,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1647,10 +1611,10 @@
         <f aca="false">"/path/from/audio/folder"</f>
         <v>/path/from/audio/folder</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="15" t="s">
         <v>95</v>
       </c>
       <c r="D2" s="20" t="s">
@@ -1659,26 +1623,26 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="14"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="14"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="14"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="14"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="22"/>
+      <c r="C7" s="15"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1709,8 +1673,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="11.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="24" width="11.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="11.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="23" width="11.84"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="4" style="1" width="11.52"/>
   </cols>
   <sheetData>
@@ -1726,13 +1690,13 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="B2" s="24" t="n">
+      <c r="B2" s="23" t="n">
         <v>0</v>
       </c>
-      <c r="C2" s="24" t="n">
+      <c r="C2" s="23" t="n">
         <v>20000</v>
       </c>
     </row>
@@ -1777,8 +1741,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="24" width="18.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="23" width="18.97"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1016" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
@@ -1791,10 +1755,10 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="B2" s="24" t="n">
+      <c r="B2" s="23" t="n">
         <v>15</v>
       </c>
     </row>
@@ -1836,8 +1800,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="24" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="23" width="14.35"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="4" style="1" width="11.52"/>
   </cols>
   <sheetData>
@@ -1853,7 +1817,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="22" t="s">
         <v>99</v>
       </c>
       <c r="B2" s="20" t="s">

</xml_diff>

<commit_message>
feat: Add `audio_host` user setting
Example: http://localhost:3000

This is the file server serving the `audio_folder`. It allows to access the files from the `front` package in order to playback audio, display waveforms and spectrograms.
</commit_message>
<xml_diff>
--- a/examples/common/config.xlsx
+++ b/examples/common/config.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="105">
   <si>
     <t xml:space="preserve">Sound Scape Explorer</t>
   </si>
@@ -43,6 +43,115 @@
   </si>
   <si>
     <t xml:space="preserve">See help below</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Settings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">base_path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The relative or absolute path to your project folder. Examples: “./relative/project” “/absolute/project”.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">audio_folder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The name of the folder containing your audio samples.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">audio_host</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">The host name serving your audio files for playbacks. Example: “</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">http://localhost:3000</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">”</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">expected_sample_rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The sample rate of your audio samples.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">umap_seed</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Optional </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">The seed number used for UMAP reductions.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">timezone</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Optional</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> The timezone of your project. If empty, dates and times will display as UTC.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Files</t>
@@ -339,80 +448,10 @@
     <t xml:space="preserve">value</t>
   </si>
   <si>
-    <t xml:space="preserve">base_path</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./project</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The relative or absolute path to your project folder. Examples: “./relative/project” “/absolute/project”.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">audio_folder</t>
-  </si>
-  <si>
     <t xml:space="preserve">audio</t>
   </si>
   <si>
-    <t xml:space="preserve">The name of the folder containing your audio samples.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">expected_sample_rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The sample rate of your audio samples.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">umap_seed</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Optional </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">The seed number used for UMAP reductions.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">timezone</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Optional</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> The timezone of your project. If empty, dates and times will display as UTC.</t>
-    </r>
+    <t xml:space="preserve">http://localhost:3000</t>
   </si>
   <si>
     <t xml:space="preserve">meta_LABEL</t>
@@ -446,7 +485,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -491,9 +530,24 @@
       <charset val="1"/>
     </font>
     <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <i val="true"/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -593,7 +647,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -622,11 +676,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -658,7 +712,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -690,7 +748,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -776,18 +834,18 @@
     <tabColor rgb="FFEEEEEE"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="I26" activeCellId="0" sqref="I26"/>
+      <selection pane="topRight" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="74.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="81.83"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
@@ -849,27 +907,27 @@
         <v>12</v>
       </c>
     </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="6" t="s">
+      <c r="A11" s="7" t="s">
         <v>15</v>
       </c>
+      <c r="B11" s="8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="6" t="s">
+      <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="B13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
@@ -879,136 +937,193 @@
         <v>19</v>
       </c>
     </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="2"/>
+      <c r="A16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>24</v>
-      </c>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="2"/>
+      <c r="A20" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>31</v>
-      </c>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25" s="2"/>
+      <c r="A25" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B28" s="8" t="s">
+      <c r="A28" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="B28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="6" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="2" t="s">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="2"/>
+      <c r="B31" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B33" s="6" t="s">
+      <c r="A33" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="B33" s="2"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B35" s="2"/>
+      <c r="A35" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>48</v>
+      <c r="A36" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" s="2"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" s="2"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:A3"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B8" r:id="rId1" display="http://localhost:3000"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1027,7 +1142,7 @@
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -1037,47 +1152,47 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="23" width="14.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="23" width="17.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="23" width="15.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="23" width="25.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="24" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="24" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="24" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="24" width="25.98"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="6" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" s="24" t="s">
-        <v>41</v>
+      <c r="A1" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>54</v>
       </c>
       <c r="F1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" s="20" t="n">
+      <c r="A2" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="21" t="n">
         <v>2</v>
       </c>
-      <c r="C2" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="E2" s="25" t="s">
-        <v>99</v>
+      <c r="C2" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1109,7 +1224,7 @@
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -1119,18 +1234,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="13.17"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="21" t="s">
-        <v>44</v>
+      <c r="A1" s="22" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="s">
-        <v>70</v>
+      <c r="A2" s="23" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1162,7 +1277,7 @@
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -1172,18 +1287,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="15.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="15.63"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="21" t="s">
-        <v>47</v>
+      <c r="A1" s="22" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="s">
-        <v>72</v>
+      <c r="A2" s="23" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1215,7 +1330,7 @@
   </sheetPr>
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -1231,27 +1346,27 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1273,7 +1388,7 @@
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -1290,82 +1405,82 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1387,7 +1502,7 @@
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -1404,42 +1519,42 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1474,89 +1589,82 @@
     <tabColor rgb="FFFFFFD7"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="94.58"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>53</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>84</v>
+        <v>5</v>
+      </c>
+      <c r="B2" s="15" t="str">
+        <f aca="false">"/path/to/your/project"</f>
+        <v>/path/to/your/project</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="B4" s="15" t="n">
+        <v>9</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="15" t="n">
         <v>44100</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="B5" s="17" t="n">
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="18" t="n">
         <v>42000</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="8" t="s">
-        <v>93</v>
-      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="18"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" display="http://localhost:3000"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1575,7 +1683,7 @@
   </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -1585,25 +1693,25 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="18" width="56.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="19" width="42.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="19" width="22.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="20" width="20.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="19" width="56.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="20" width="22.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="21" width="20.56"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1009" min="5" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>94</v>
+        <v>20</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1612,13 +1720,13 @@
         <v>/path/from/audio/folder</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>96</v>
+        <v>98</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1663,54 +1771,54 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="L1" activeCellId="0" sqref="L1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="11.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="23" width="11.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="11.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="24" width="11.84"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="4" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="21" t="s">
-        <v>18</v>
+      <c r="A1" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="B2" s="23" t="n">
+      <c r="A2" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="24" t="n">
         <v>0</v>
       </c>
-      <c r="C2" s="23" t="n">
+      <c r="C2" s="24" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1731,7 +1839,7 @@
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -1741,35 +1849,35 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="23" width="18.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="24" width="18.97"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1016" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>23</v>
+      <c r="A1" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="B2" s="23" t="n">
+      <c r="A2" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="24" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="20"/>
+      <c r="B4" s="21"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="20"/>
+      <c r="B5" s="21"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="20"/>
+      <c r="B6" s="21"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1790,7 +1898,7 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -1800,39 +1908,39 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="23" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="24" width="14.35"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="4" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="21" t="s">
-        <v>30</v>
+      <c r="A1" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>101</v>
+      <c r="A2" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="20"/>
+      <c r="C4" s="21"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
feat: Add `audio` package for hosting audio files + Improve `front` player + Add `front` `indicators` and `volumes` Improve and clean code and builds
</commit_message>
<xml_diff>
--- a/examples/common/config.xlsx
+++ b/examples/common/config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Help" sheetId="1" state="visible" r:id="rId2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="104">
   <si>
     <t xml:space="preserve">Sound Scape Explorer</t>
   </si>
@@ -61,39 +61,6 @@
   </si>
   <si>
     <t xml:space="preserve">audio_host</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">The host name serving your audio files for playbacks. Example: “</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">http://localhost:3000</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">”</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">expected_sample_rate</t>
@@ -482,10 +449,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -525,14 +493,6 @@
     <font>
       <i val="true"/>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -676,11 +636,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -708,15 +668,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -748,7 +708,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -836,10 +796,10 @@
   </sheetPr>
   <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B10" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topRight" activeCell="A37" activeCellId="0" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -895,235 +855,233 @@
       <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>10</v>
+      <c r="B8" s="6" t="str">
+        <f aca="false">"The host name serving your audio files. For Docker, use 'http://localhost:3000'"</f>
+        <v>The host name serving your audio files. For Docker, use 'http://localhost:3000'</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>11</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>13</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>18</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>20</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>27</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="6" t="s">
         <v>39</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B33" s="2"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" s="8" t="s">
         <v>50</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="8" t="s">
         <v>52</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38" s="8" t="s">
         <v>54</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B40" s="2"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B41" s="6" t="s">
         <v>57</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B43" s="2"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B44" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:A3"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1" display="http://localhost:3000"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1162,37 +1120,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" s="21" t="n">
         <v>2</v>
       </c>
       <c r="C2" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="E2" s="26" t="s">
         <v>101</v>
-      </c>
-      <c r="E2" s="26" t="s">
-        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1240,12 +1198,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1293,12 +1251,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1346,27 +1304,27 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1405,82 +1363,82 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>67</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>69</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>71</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>73</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="12" t="s">
         <v>75</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>77</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>79</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1519,42 +1477,42 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>85</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>87</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>89</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>91</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1591,7 +1549,7 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -1608,10 +1566,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>93</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1628,7 +1586,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1636,12 +1594,12 @@
         <v>9</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="15" t="n">
         <v>44100</v>
@@ -1649,7 +1607,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="18" t="n">
         <v>42000</v>
@@ -1657,7 +1615,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="18"/>
     </row>
@@ -1702,16 +1660,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1720,13 +1678,13 @@
         <v>/path/from/audio/folder</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="21" t="s">
         <v>98</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1788,18 +1746,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B2" s="24" t="n">
         <v>0</v>
@@ -1856,15 +1814,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B2" s="24" t="n">
         <v>15</v>
@@ -1915,24 +1873,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="C2" s="21" t="s">
         <v>103</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
chore(Config): Clean configuration file
</commit_message>
<xml_diff>
--- a/examples/common/config.xlsx
+++ b/examples/common/config.xlsx
@@ -796,10 +796,10 @@
   </sheetPr>
   <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B10" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
-      <selection pane="topRight" activeCell="A37" activeCellId="0" sqref="A37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -856,8 +856,8 @@
         <v>9</v>
       </c>
       <c r="B8" s="6" t="str">
-        <f aca="false">"The host name serving your audio files. For Docker, use 'http://localhost:3000'"</f>
-        <v>The host name serving your audio files. For Docker, use 'http://localhost:3000'</v>
+        <f aca="false">"The host name serving your audio files. For Docker, use 'http://localhost:3000'."</f>
+        <v>The host name serving your audio files. For Docker, use 'http://localhost:3000'.</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1554,7 +1554,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1646,7 +1646,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
feat: Add optional `autocluster` user setting + Fix `yarn process:autocluster` command + Update example configuration file
</commit_message>
<xml_diff>
--- a/examples/common/config.xlsx
+++ b/examples/common/config.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="107">
   <si>
     <t xml:space="preserve">Sound Scape Explorer</t>
   </si>
@@ -51,7 +51,7 @@
     <t xml:space="preserve">base_path</t>
   </si>
   <si>
-    <t xml:space="preserve">The relative or absolute path to your project folder. Examples: “./relative/project” “/absolute/project”.</t>
+    <t xml:space="preserve">The relative or absolute path to your project folder. Examples: `./relative/project` `/absolute/project`.</t>
   </si>
   <si>
     <t xml:space="preserve">audio_folder</t>
@@ -121,6 +121,32 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">autocluster</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Optional</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Whether you want to run auto clustering process. `yes` or `no`.</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">Files</t>
   </si>
   <si>
@@ -419,6 +445,9 @@
   </si>
   <si>
     <t xml:space="preserve">http://localhost:3000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
   </si>
   <si>
     <t xml:space="preserve">meta_LABEL</t>
@@ -794,12 +823,12 @@
     <tabColor rgb="FFEEEEEE"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B44"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -884,19 +913,19 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B12" s="8" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="6" t="s">
+      <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="B14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
@@ -922,19 +951,19 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="2"/>
+      <c r="B18" s="6" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="6" t="s">
+      <c r="A20" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="B20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
@@ -952,19 +981,19 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2" t="s">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="2"/>
+      <c r="B23" s="6" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25" s="6" t="s">
+      <c r="A25" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="B25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
@@ -974,19 +1003,19 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="s">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="2"/>
+      <c r="B27" s="6" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29" s="6" t="s">
+      <c r="A29" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="B29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
@@ -1004,19 +1033,19 @@
         <v>43</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="2" t="s">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B33" s="2"/>
+      <c r="B32" s="6" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B34" s="6" t="s">
+      <c r="A34" s="2" t="s">
         <v>46</v>
       </c>
+      <c r="B34" s="2"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="s">
@@ -1027,10 +1056,10 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="6" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1050,32 +1079,40 @@
         <v>54</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="2" t="s">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B40" s="2"/>
+      <c r="B39" s="8" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B41" s="6" t="s">
+      <c r="A41" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="2" t="s">
+      <c r="B41" s="2"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B43" s="2"/>
+      <c r="B42" s="6" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B44" s="6" t="s">
+      <c r="A44" s="2" t="s">
         <v>60</v>
+      </c>
+      <c r="B44" s="2"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1120,37 +1157,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B2" s="21" t="n">
         <v>2</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1198,12 +1235,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1240,7 +1277,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1251,12 +1288,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1304,27 +1341,27 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1363,82 +1400,82 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1477,42 +1514,42 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1547,14 +1584,14 @@
     <tabColor rgb="FFFFFFD7"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1566,10 +1603,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1586,7 +1623,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1594,7 +1631,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1618,6 +1655,14 @@
         <v>14</v>
       </c>
       <c r="B7" s="18"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>98</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1660,16 +1705,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B1" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="13" t="s">
-        <v>19</v>
-      </c>
       <c r="D1" s="22" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1678,13 +1723,13 @@
         <v>/path/from/audio/folder</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1746,18 +1791,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B2" s="24" t="n">
         <v>0</v>
@@ -1814,15 +1859,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B2" s="24" t="n">
         <v>15</v>
@@ -1873,24 +1918,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
feat(Processing): Add matrices and pairings to configuration file.
Rename `ClusterPairing` to `ContingencyPairing`

BREAKING CHANGE: Configuration file has changed, matrices and pairings
options have been added.
</commit_message>
<xml_diff>
--- a/examples/common/config.xlsx
+++ b/examples/common/config.xlsx
@@ -12,14 +12,18 @@
     <sheet name="HelpReducers" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="HelpIndicators" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="HelpVolumes" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Settings" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Files" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Bands" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="Integrations" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="Ranges" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="Reducers" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="Indicators" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="Volumes" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="HelpMatrices" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="HelpPairings" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Settings" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Files" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Bands" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Integrations" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Ranges" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="Reducers" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="Indicators" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="Volumes" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="Matrices" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="Pairings" sheetId="16" state="visible" r:id="rId17"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -31,11 +35,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="131">
   <si>
     <t xml:space="preserve">Sound Scape Explorer</t>
   </si>
   <si>
+    <t xml:space="preserve">Version 9</t>
+  </si>
+  <si>
     <t xml:space="preserve">Instructions</t>
   </si>
   <si>
@@ -43,6 +50,29 @@
   </si>
   <si>
     <t xml:space="preserve">See help below</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Find documentation here: </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://github.com/sound-scape-explorer/sound-scape-explorer#readme</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Settings</t>
@@ -147,106 +177,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Files</t>
-  </si>
-  <si>
-    <t xml:space="preserve">file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The file path, relative to your `audio_folder`. Must start with `/`.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The file date. Format `YYYYMMDD HHMM`.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">site</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The site.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">meta_X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The meta properties. Rename `X` and add your metas.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bands</t>
-  </si>
-  <si>
-    <t xml:space="preserve">band</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The band name.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">low</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The low frequency.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">high</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The high frequency.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Integrations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">integration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The integration name.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">seconds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of seconds.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ranges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">range</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The range name.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The start date. Format `YYYYMMDD HHMM`.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">end</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The end date. Format `YYYYMMDD HHMM`.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reducers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reducer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The reducer. See `HelpReducers` tab for available options.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dimensions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of dimensions to reduce to.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bands</t>
+    <t xml:space="preserve">autocluster_iterations</t>
   </si>
   <si>
     <r>
@@ -268,11 +199,11 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> The list of band names to consider. Separate with `,`.</t>
+      <t xml:space="preserve"> The number of iterations during the autoclustering process.</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">integrations</t>
+    <t xml:space="preserve">autocluster_min_size</t>
   </si>
   <si>
     <r>
@@ -294,11 +225,11 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> The list of integration names to consider. Separate with `,`.</t>
+      <t xml:space="preserve"> The minimum expected size of clusters.</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">ranges</t>
+    <t xml:space="preserve">autocluster_max_size</t>
   </si>
   <si>
     <r>
@@ -320,10 +251,213 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> The list of range names to consider. Separate with `,`.</t>
+      <t xml:space="preserve"> The maximum expected size of clusters.</t>
     </r>
   </si>
   <si>
+    <t xml:space="preserve">autocluster_threshold</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Optional</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> The threshold to specify membership of given element in a cluster.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Files</t>
+  </si>
+  <si>
+    <t xml:space="preserve">file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The file path, relative to your `audio_folder`. Must start with `/`.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The file date. Format `YYYYMMDD HHMM`.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The site.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meta_X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The meta properties. Rename `X` and add your metas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">band</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The band name.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">low</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The low frequency.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">high</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The high frequency.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integrations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">integration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The integration name.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">seconds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of seconds.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ranges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The range name.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The start date. Format `YYYYMMDD HHMM`.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The end date. Format `YYYYMMDD HHMM`.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reducers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reducer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The reducer. See `HelpReducers` tab for available options.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dimensions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of dimensions to reduce to.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bands</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Optional</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> The list of band names to consider. Separate with `,`. If empty, all bands will be processed.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">integrations</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Optional</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> The list of integration names to consider. Separate with `,`. If empty, all integrations will be processed.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ranges</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Optional</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> The list of range names to consider. Separate with `,`. If empty, all ranges will be processed.</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">Indicators</t>
   </si>
   <si>
@@ -342,6 +476,24 @@
     <t xml:space="preserve">The indicator. See `HelpVolumes` tab for available options.</t>
   </si>
   <si>
+    <t xml:space="preserve">Matrices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">matrix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The matrix. See `HelpMatrices` tab for available options.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pairings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pairing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The pairing. See `HelpPairings` tab for available options.</t>
+  </si>
+  <si>
     <t xml:space="preserve">umap</t>
   </si>
   <si>
@@ -433,6 +585,30 @@
   </si>
   <si>
     <t xml:space="preserve">The mean spreading.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">distance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The distance between subtypes of a given cluster.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">overlap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The overlap between subtypes of a given cluster.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">silhouette</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The silhouette between subtypes of a given cluster.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contingency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contingency between two clusters.</t>
   </si>
   <si>
     <t xml:space="preserve">setting</t>
@@ -482,7 +658,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -520,6 +696,15 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
       <i val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
@@ -527,7 +712,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
       <i val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
@@ -636,7 +820,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -661,7 +845,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -673,6 +857,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -685,7 +873,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -701,18 +889,18 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -737,11 +925,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -823,18 +1011,18 @@
     <tabColor rgb="FFEEEEEE"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:B56"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topRight" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="81.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="90.96"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
@@ -842,35 +1030,35 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3"/>
       <c r="B3" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3"/>
+      <c r="B4" s="4" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="B6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
@@ -884,24 +1072,24 @@
       <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="6" t="str">
+      <c r="B8" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="6" t="str">
         <f aca="false">"The host name serving your audio files. For Docker, use 'http://localhost:3000'."</f>
         <v>The host name serving your audio files. For Docker, use 'http://localhost:3000'.</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="6" t="s">
         <v>13</v>
       </c>
     </row>
@@ -921,204 +1109,275 @@
         <v>17</v>
       </c>
     </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="2"/>
+      <c r="A14" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>20</v>
+      <c r="A15" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>22</v>
+      <c r="A16" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="6" t="s">
+      <c r="A17" s="7" t="s">
         <v>26</v>
       </c>
+      <c r="B17" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="2"/>
+      <c r="A20" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B29" s="2"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>41</v>
-      </c>
+      <c r="A30" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" s="2"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B34" s="2"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B38" s="8" t="s">
+      <c r="A37" s="5" t="s">
         <v>54</v>
       </c>
+      <c r="B37" s="6" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B39" s="8" t="s">
+      <c r="A39" s="2" t="s">
         <v>56</v>
       </c>
+      <c r="B39" s="2"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B41" s="2"/>
+      <c r="A41" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>59</v>
+      <c r="A42" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B44" s="2"/>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>62</v>
+      <c r="A44" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B46" s="2"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B49" s="2"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B52" s="2"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B55" s="2"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A2:A4"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" location="readme" display="https://github.com/sound-scape-explorer/sound-scape-explorer#readme"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1130,6 +1389,128 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <tabColor rgb="FFFFFFD7"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="24" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="18.97"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1016" min="3" style="1" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" s="25" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="22"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="22"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="22"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <tabColor rgb="FFFFFFD7"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="24" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="25" width="14.35"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="4" style="1" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="22"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFD7"/>
@@ -1147,47 +1528,47 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="24" width="14.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="24" width="17.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="24" width="15.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="24" width="25.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="24" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="25" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="25" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="25" width="25.98"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="6" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="D1" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="E1" s="25" t="s">
-        <v>55</v>
+      <c r="A1" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>65</v>
       </c>
       <c r="F1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2" s="21" t="n">
+      <c r="A2" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="22" t="n">
         <v>2</v>
       </c>
-      <c r="C2" s="26" t="s">
-        <v>102</v>
-      </c>
-      <c r="D2" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="E2" s="26" t="s">
-        <v>104</v>
+      <c r="C2" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1211,7 +1592,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFD7"/>
@@ -1229,18 +1610,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="24" width="13.17"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="22" t="s">
-        <v>58</v>
+      <c r="A1" s="23" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23" t="s">
-        <v>84</v>
+      <c r="A2" s="24" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1264,7 +1645,119 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <tabColor rgb="FFFFFFD7"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="24" width="15.63"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="24" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1002" type="list">
+      <formula1>HelpVolumes!$A$2:$A$1048576</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1" type="none">
+      <formula1>HelpVolumes!$A$2:$A$1048576</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <tabColor rgb="FFFFFFD7"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A6" activeCellId="0" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="24" width="15.63"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="24" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="24" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="24" t="s">
+        <v>114</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1:A1004" type="list">
+      <formula1>HelpMatrices!$A$2:$A$1048576</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFD7"/>
@@ -1282,28 +1775,24 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="15.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="24" width="15.63"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="22" t="s">
-        <v>61</v>
+      <c r="A1" s="23" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23" t="s">
-        <v>86</v>
+      <c r="A2" s="24" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1002" type="list">
-      <formula1>HelpVolumes!$A$2:$A$1048576</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1" type="none">
-      <formula1>HelpVolumes!$A$2:$A$1048576</formula1>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1:A1001" type="list">
+      <formula1>HelpPairings!$A$2:$A$1048576</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -1335,33 +1824,33 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="9" width="16.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="16.24"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10" t="s">
-        <v>47</v>
+      <c r="A1" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
-        <v>63</v>
+      <c r="A2" s="10" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
-        <v>64</v>
+      <c r="A3" s="10" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
-        <v>65</v>
+      <c r="A4" s="10" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
-        <v>66</v>
+      <c r="A5" s="10" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1393,89 +1882,89 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="9" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="12" width="42.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10" t="s">
-        <v>58</v>
+      <c r="A1" s="11" t="s">
+        <v>68</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>69</v>
+      <c r="A2" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>71</v>
+      <c r="A3" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>73</v>
+      <c r="A4" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>75</v>
+      <c r="A5" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>77</v>
+      <c r="A6" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>79</v>
+      <c r="A7" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>81</v>
+      <c r="A8" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>83</v>
+      <c r="A9" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>85</v>
+      <c r="A10" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1507,65 +1996,65 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="9" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="12" width="42.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10" t="s">
-        <v>61</v>
+      <c r="A1" s="11" t="s">
+        <v>71</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>87</v>
+      <c r="A2" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>89</v>
+      <c r="A3" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>91</v>
+      <c r="A4" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>93</v>
+      <c r="A5" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="12"/>
+      <c r="B6" s="13"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="6"/>
+      <c r="B7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="6"/>
+      <c r="B8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="6"/>
+      <c r="B9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="6"/>
+      <c r="B10" s="9"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1581,17 +2070,175 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
-    <tabColor rgb="FFFFFFD7"/>
+    <tabColor rgb="FFEEEEEE"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="12" width="42.79"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="13"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="13"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="9"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="9"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="9"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="9"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <tabColor rgb="FFEEEEEE"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="12" width="42.79"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="13"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="13"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="13"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="13"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="9"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="9"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="9"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="9"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <tabColor rgb="FFFFFFD7"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1602,66 +2249,98 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>95</v>
+      <c r="A1" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="15" t="str">
+      <c r="A2" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="16" t="str">
         <f aca="false">"/path/to/your/project"</f>
         <v>/path/to/your/project</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>96</v>
+      <c r="A3" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>97</v>
+      <c r="A4" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="15" t="n">
+      <c r="A5" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="16" t="n">
         <v>44100</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="18" t="n">
+      <c r="A6" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="19" t="n">
         <v>42000</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="18"/>
+      <c r="A7" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="19"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>98</v>
+      <c r="A8" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="19" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="19" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="19" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="19" t="n">
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>
@@ -1678,7 +2357,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFD7"/>
@@ -1696,191 +2375,64 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="19" width="56.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="42.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="20" width="22.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="21" width="20.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="20" width="56.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="21" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="21" width="22.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="22" width="20.56"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1009" min="5" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>99</v>
+      <c r="A1" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="14" t="str">
+      <c r="A2" s="15" t="str">
         <f aca="false">"/path/from/audio/folder"</f>
         <v>/path/from/audio/folder</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>101</v>
+      <c r="B2" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="14"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="14"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
+      <c r="A4" s="15"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="14"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="14"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="15"/>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <tabColor rgb="FFFFFFD7"/>
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="11.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="24" width="11.84"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="4" style="1" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="B2" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" s="24" t="n">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <tabColor rgb="FFFFFFD7"/>
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="24" width="18.97"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1016" min="3" style="1" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="22" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="B2" s="24" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="21"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="21"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="21"/>
+      <c r="C7" s="16"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1899,51 +2451,56 @@
     <tabColor rgb="FFFFFFD7"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="24" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="24" width="11.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="25" width="11.84"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="4" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="C1" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="22" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
+      <c r="A2" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" s="25" t="n">
+        <v>20</v>
+      </c>
+      <c r="C2" s="25" t="n">
+        <v>20000</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="21"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
feat(Processing/Config): Add UMAP optional settings with defaults
</commit_message>
<xml_diff>
--- a/examples/common/config.xlsx
+++ b/examples/common/config.xlsx
@@ -9,21 +9,22 @@
   </bookViews>
   <sheets>
     <sheet name="Help" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="HelpReducers" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="HelpIndicators" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="HelpVolumes" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="HelpMatrices" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="HelpPairings" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Settings" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="Files" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="Bands" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="Integrations" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="Ranges" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="Reducers" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="Indicators" sheetId="13" state="visible" r:id="rId14"/>
-    <sheet name="Volumes" sheetId="14" state="visible" r:id="rId15"/>
-    <sheet name="Matrices" sheetId="15" state="visible" r:id="rId16"/>
-    <sheet name="Pairings" sheetId="16" state="visible" r:id="rId17"/>
+    <sheet name="HelpSettings" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="HelpReducers" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="HelpIndicators" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="HelpVolumes" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="HelpMatrices" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="HelpPairings" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Settings" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Files" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Bands" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Integrations" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="Ranges" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="Reducers" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="Indicators" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="Volumes" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="Matrices" sheetId="16" state="visible" r:id="rId17"/>
+    <sheet name="Pairings" sheetId="17" state="visible" r:id="rId18"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="158">
   <si>
     <t xml:space="preserve">Sound Scape Explorer</t>
   </si>
@@ -52,51 +53,79 @@
     <t xml:space="preserve">See help below</t>
   </si>
   <si>
+    <t xml:space="preserve">Find documentation here: https://github.com/sound-scape-explorer/sound-scape-explorer#readme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Settings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">base_path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The relative or absolute path to your project folder. Examples: `./relative/project` `/absolute/project`.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">audio_folder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The name of the folder containing your audio samples.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">audio_host</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expected_sample_rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The sample rate of your audio samples.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">timezone</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b val="true"/>
+        <i val="true"/>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Find documentation here: </t>
+      <t xml:space="preserve">Optional</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> The timezone of your project. If empty, dates and times will display as UTC.
+</t>
     </r>
     <r>
       <rPr>
         <b val="true"/>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
+        <i val="true"/>
+        <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">https://github.com/sound-scape-explorer/sound-scape-explorer#readme</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Settings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">base_path</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The relative or absolute path to your project folder. Examples: `./relative/project` `/absolute/project`.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">audio_folder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The name of the folder containing your audio samples.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">audio_host</t>
-  </si>
-  <si>
-    <t xml:space="preserve">expected_sample_rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The sample rate of your audio samples.</t>
+      <t xml:space="preserve">Default</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> None</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">umap_seed</t>
@@ -121,13 +150,9 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">The seed number used for UMAP reductions.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">timezone</t>
-  </si>
-  <si>
+      <t xml:space="preserve">The seed number used for UMAP reductions. Also used for PCA based reductions.
+</t>
+    </r>
     <r>
       <rPr>
         <b val="true"/>
@@ -135,8 +160,124 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Default</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> None</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">umap_neighbors</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
         <charset val="1"/>
       </rPr>
+      <t xml:space="preserve">Optional </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">The size of local neighborhood used for UMAP.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Default</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 15</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">umap_metric</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Optional </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">The metric to use to compute distances in high dimensional space.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Default</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> euclidean</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">autocluster</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">Optional</t>
     </r>
     <r>
@@ -147,13 +288,9 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> The timezone of your project. If empty, dates and times will display as UTC.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">autocluster</t>
-  </si>
-  <si>
+      <t xml:space="preserve"> Whether you want to run auto clustering process. `yes` or `no`.
+</t>
+    </r>
     <r>
       <rPr>
         <b val="true"/>
@@ -161,6 +298,30 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Default</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> False</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">autocluster_iterations</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Optional</t>
@@ -173,13 +334,9 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> Whether you want to run auto clustering process. `yes` or `no`.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">autocluster_iterations</t>
-  </si>
-  <si>
+      <t xml:space="preserve"> The number of iterations during the autoclustering process.
+</t>
+    </r>
     <r>
       <rPr>
         <b val="true"/>
@@ -187,6 +344,30 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Default</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 100</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">autocluster_min_size</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Optional</t>
@@ -199,13 +380,9 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> The number of iterations during the autoclustering process.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">autocluster_min_size</t>
-  </si>
-  <si>
+      <t xml:space="preserve"> The minimum expected size of clusters.
+</t>
+    </r>
     <r>
       <rPr>
         <b val="true"/>
@@ -213,6 +390,30 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Default</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 20</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">autocluster_max_size</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Optional</t>
@@ -225,13 +426,9 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> The minimum expected size of clusters.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">autocluster_max_size</t>
-  </si>
-  <si>
+      <t xml:space="preserve"> The maximum expected size of clusters.
+</t>
+    </r>
     <r>
       <rPr>
         <b val="true"/>
@@ -239,6 +436,30 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Default</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 60</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">autocluster_threshold</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Optional</t>
@@ -251,13 +472,9 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> The maximum expected size of clusters.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">autocluster_threshold</t>
-  </si>
-  <si>
+      <t xml:space="preserve"> The threshold to specify membership of given element in a cluster.
+</t>
+    </r>
     <r>
       <rPr>
         <b val="true"/>
@@ -265,6 +482,129 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Default</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 0.9</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Files</t>
+  </si>
+  <si>
+    <t xml:space="preserve">file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The file path, relative to your `audio_folder`. Must start with `/`.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The file date. Format `YYYYMMDD HHMM`.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The site.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meta_X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The meta properties. Rename `X` and add your metas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">band</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The band name.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">low</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The low frequency.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">high</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The high frequency.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integrations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">integration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The integration name.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">seconds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of seconds.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ranges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The range name.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The start date. Format `YYYYMMDD HHMM`.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The end date. Format `YYYYMMDD HHMM`.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reducers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reducer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The reducer. See `HelpReducers` tab for available options.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dimensions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of dimensions to reduce to.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bands</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Optional</t>
@@ -277,110 +617,11 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> The threshold to specify membership of given element in a cluster.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Files</t>
-  </si>
-  <si>
-    <t xml:space="preserve">file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The file path, relative to your `audio_folder`. Must start with `/`.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The file date. Format `YYYYMMDD HHMM`.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">site</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The site.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">meta_X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The meta properties. Rename `X` and add your metas.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bands</t>
-  </si>
-  <si>
-    <t xml:space="preserve">band</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The band name.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">low</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The low frequency.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">high</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The high frequency.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Integrations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">integration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The integration name.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">seconds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of seconds.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ranges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">range</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The range name.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The start date. Format `YYYYMMDD HHMM`.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">end</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The end date. Format `YYYYMMDD HHMM`.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reducers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reducer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The reducer. See `HelpReducers` tab for available options.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dimensions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of dimensions to reduce to.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bands</t>
+      <t xml:space="preserve"> The list of band names to consider. Separate with `,`. If empty, all bands will be processed.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">integrations</t>
   </si>
   <si>
     <r>
@@ -402,11 +643,11 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> The list of band names to consider. Separate with `,`. If empty, all bands will be processed.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">integrations</t>
+      <t xml:space="preserve"> The list of integration names to consider. Separate with `,`. If empty, all integrations will be processed.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ranges</t>
   </si>
   <si>
     <r>
@@ -428,32 +669,6 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> The list of integration names to consider. Separate with `,`. If empty, all integrations will be processed.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">ranges</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Optional</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
       <t xml:space="preserve"> The list of range names to consider. Separate with `,`. If empty, all ranges will be processed.</t>
     </r>
   </si>
@@ -492,6 +707,75 @@
   </si>
   <si>
     <t xml:space="preserve">The pairing. See `HelpPairings` tab for available options.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">euclidean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">manhattan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chebyshev</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minkowski</t>
+  </si>
+  <si>
+    <t xml:space="preserve">canberra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">braycurtis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mahalanobis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wminkowski</t>
+  </si>
+  <si>
+    <t xml:space="preserve">seuclidean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cosine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">correlation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">haversine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hamming</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jaccard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">russelrao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kulsinski</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ll_dirichlet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hellinger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rogerstanimoto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sokalmichener</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sokalsneath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yule</t>
   </si>
   <si>
     <t xml:space="preserve">umap</t>
@@ -658,7 +942,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -717,6 +1001,19 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <i val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -820,7 +1117,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -841,6 +1138,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -850,11 +1151,15 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -889,7 +1194,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -925,7 +1230,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1011,12 +1316,12 @@
     <tabColor rgb="FFEEEEEE"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B56"/>
+  <dimension ref="A1:B58"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topRight" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1050,7 +1355,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3"/>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1061,314 +1366,330 @@
       <c r="B6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="6" t="str">
+      <c r="B9" s="7" t="str">
         <f aca="false">"The host name serving your audio files. For Docker, use 'http://localhost:3000'."</f>
         <v>The host name serving your audio files. For Docker, use 'http://localhost:3000'.</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="s">
+    <row r="11" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
+    <row r="12" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="s">
+    <row r="13" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="s">
+    <row r="14" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="s">
+    <row r="15" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="s">
+    <row r="16" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="s">
+    <row r="17" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
+    <row r="18" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="2"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5" t="s">
+      <c r="B18" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="6" t="s">
+    </row>
+    <row r="19" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="8" t="s">
         <v>30</v>
       </c>
+      <c r="B19" s="9" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="6" t="s">
+      <c r="A21" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="B21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="7" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="7" t="s">
         <v>36</v>
       </c>
     </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B25" s="2"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="6" t="s">
+      <c r="A25" s="6" t="s">
         <v>39</v>
       </c>
+      <c r="B25" s="7" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B27" s="6" t="s">
+      <c r="A27" s="2" t="s">
         <v>41</v>
       </c>
+      <c r="B27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="7" t="s">
         <v>43</v>
       </c>
     </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B30" s="2"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B31" s="6" t="s">
+      <c r="A30" s="6" t="s">
         <v>46</v>
       </c>
+      <c r="B30" s="7" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B32" s="6" t="s">
+      <c r="A32" s="2" t="s">
         <v>48</v>
       </c>
+      <c r="B32" s="2"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B34" s="2"/>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B35" s="6" t="s">
+      <c r="A34" s="6" t="s">
         <v>51</v>
       </c>
+      <c r="B34" s="7" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B36" s="6" t="s">
+      <c r="A36" s="2" t="s">
         <v>53</v>
       </c>
+      <c r="B36" s="2"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="7" t="s">
         <v>55</v>
       </c>
     </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B39" s="2"/>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B40" s="6" t="s">
+      <c r="A39" s="6" t="s">
         <v>58</v>
       </c>
+      <c r="B39" s="7" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B41" s="6" t="s">
+      <c r="A41" s="2" t="s">
         <v>60</v>
       </c>
+      <c r="B41" s="2"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="7" t="s">
+      <c r="A42" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="B42" s="7" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="7" t="s">
+      <c r="A43" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="B43" s="7" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="7" t="s">
+      <c r="A44" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="B44" s="9" t="s">
         <v>66</v>
       </c>
     </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B46" s="2"/>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B47" s="9" t="s">
+      <c r="A46" s="10" t="s">
         <v>69</v>
       </c>
+      <c r="B46" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B48" s="2"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B49" s="2"/>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B50" s="9" t="s">
+      <c r="A49" s="6" t="s">
         <v>72</v>
       </c>
+      <c r="B49" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B51" s="2"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B52" s="2"/>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B53" s="9" t="s">
+      <c r="A52" s="6" t="s">
         <v>75</v>
       </c>
+      <c r="B52" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B54" s="2"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B55" s="2"/>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B56" s="9" t="s">
+      <c r="A55" s="6" t="s">
         <v>78</v>
+      </c>
+      <c r="B55" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B57" s="2"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B58" s="11" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1376,7 +1697,7 @@
     <mergeCell ref="A2:A4"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" location="readme" display="https://github.com/sound-scape-explorer/sound-scape-explorer#readme"/>
+    <hyperlink ref="B4" r:id="rId1" location="readme" display="Find documentation here: https://github.com/sound-scape-explorer/sound-scape-explorer#readme"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1394,47 +1715,56 @@
     <tabColor rgb="FFFFFFD7"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="24" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="18.97"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1016" min="3" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="11.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="27" width="11.84"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="4" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="23" t="s">
-        <v>47</v>
+      <c r="A1" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="B2" s="25" t="n">
-        <v>15</v>
+      <c r="A2" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="B2" s="27" t="n">
+        <v>20</v>
+      </c>
+      <c r="C2" s="27" t="n">
+        <v>20000</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="22"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="22"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="22"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1453,7 +1783,7 @@
     <tabColor rgb="FFFFFFD7"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -1465,39 +1795,35 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="24" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="25" width="14.35"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="4" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="27" width="18.97"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1016" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B1" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" s="23" t="s">
-        <v>54</v>
+      <c r="A1" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
+      <c r="A2" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2" s="27" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="22"/>
+      <c r="B4" s="24"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="24"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="24"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1516,7 +1842,7 @@
     <tabColor rgb="FFFFFFD7"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -1528,60 +1854,41 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="24" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="14.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="25" width="17.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="25" width="15.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="25" width="25.98"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="6" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="27" width="14.35"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="4" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="B1" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="D1" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="E1" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="F1" s="0"/>
+      <c r="A1" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="B2" s="22" t="n">
-        <v>2</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>127</v>
-      </c>
-      <c r="E2" s="27" t="s">
-        <v>128</v>
-      </c>
+      <c r="A2" s="26" t="s">
+        <v>155</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="24"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1002" type="list">
-      <formula1>HelpReducers!$A$2:$A$1048576</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1" type="none">
-      <formula1>HelpReducers!$A$2:$A$1048576</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1598,7 +1905,7 @@
     <tabColor rgb="FFFFFFD7"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -1610,28 +1917,57 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="24" width="13.17"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="27" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="27" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="27" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="27" width="25.98"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="6" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23" t="s">
-        <v>68</v>
-      </c>
+      <c r="A1" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="24" t="s">
-        <v>100</v>
+      <c r="A2" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>153</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1002" type="list">
-      <formula1>HelpIndicators!$A$2:$A$1048576</formula1>
+      <formula1>HelpReducers!$A$2:$A$1048576</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1" type="none">
-      <formula1>HelpIndicators!$A$2:$A$1048576</formula1>
+      <formula1>HelpReducers!$A$2:$A$1048576</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -1658,23 +1994,76 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="13.17"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="26" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1002" type="list">
+      <formula1>HelpIndicators!$A$2:$A$1048576</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1" type="none">
+      <formula1>HelpIndicators!$A$2:$A$1048576</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <tabColor rgb="FFFFFFD7"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="24" width="15.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="15.63"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23" t="s">
-        <v>71</v>
+      <c r="A1" s="25" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="24" t="s">
-        <v>102</v>
+      <c r="A2" s="26" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1698,7 +2087,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFD7"/>
@@ -1716,28 +2105,28 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="24" width="15.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="15.63"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23" t="s">
-        <v>74</v>
+      <c r="A1" s="25" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="24" t="s">
-        <v>110</v>
+      <c r="A2" s="26" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="24" t="s">
-        <v>112</v>
+      <c r="A3" s="26" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="24" t="s">
-        <v>114</v>
+      <c r="A4" s="26" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1757,7 +2146,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFD7"/>
@@ -1775,18 +2164,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="24" width="15.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="15.63"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23" t="s">
-        <v>77</v>
+      <c r="A1" s="25" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="24" t="s">
-        <v>116</v>
+      <c r="A2" s="26" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1812,7 +2201,7 @@
     <tabColor rgb="FFEEEEEE"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -1824,33 +2213,128 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="16.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="16.24"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
-        <v>57</v>
+      <c r="A1" s="13" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
-        <v>79</v>
+      <c r="A2" s="12" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="s">
-        <v>80</v>
+      <c r="A3" s="12" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="s">
-        <v>81</v>
+      <c r="A4" s="12" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="s">
-        <v>82</v>
+      <c r="A5" s="12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="12" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1870,7 +2354,7 @@
     <tabColor rgb="FFEEEEEE"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -1882,89 +2366,33 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="12" width="42.79"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="16.24"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>83</v>
+      <c r="A1" s="13" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>85</v>
+      <c r="A2" s="12" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>87</v>
+      <c r="A3" s="12" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>89</v>
+      <c r="A4" s="12" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>101</v>
+      <c r="A5" s="12" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1996,65 +2424,90 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="12" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="42.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
-        <v>71</v>
+      <c r="A1" s="13" t="s">
+        <v>72</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>83</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>103</v>
+      <c r="A2" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>105</v>
+      <c r="A3" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>107</v>
+      <c r="A4" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>109</v>
+      <c r="A5" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="13"/>
+      <c r="A6" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="9"/>
+      <c r="A7" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="9"/>
+      <c r="A8" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="9"/>
+      <c r="A9" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="9"/>
+      <c r="A10" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>128</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2080,65 +2533,70 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="12" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="42.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
-        <v>74</v>
+      <c r="A1" s="13" t="s">
+        <v>75</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>83</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>111</v>
+      <c r="A2" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>113</v>
+      <c r="A3" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>115</v>
+      <c r="A4" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="13"/>
+      <c r="A5" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="13"/>
+      <c r="B6" s="15"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="9"/>
+      <c r="B7" s="11"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="9"/>
+      <c r="B8" s="11"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="9"/>
+      <c r="B9" s="11"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="9"/>
+      <c r="B10" s="11"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2164,55 +2622,65 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="12" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="42.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
-        <v>74</v>
+      <c r="A1" s="13" t="s">
+        <v>78</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>83</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>117</v>
+      <c r="A2" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="13"/>
+      <c r="A3" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="13"/>
+      <c r="A4" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="13"/>
+      <c r="B5" s="15"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="13"/>
+      <c r="B6" s="15"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="9"/>
+      <c r="B7" s="11"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="9"/>
+      <c r="B8" s="11"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="9"/>
+      <c r="B9" s="11"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="9"/>
+      <c r="B10" s="11"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2228,17 +2696,91 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
-    <tabColor rgb="FFFFFFD7"/>
+    <tabColor rgb="FFEEEEEE"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="42.79"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="15"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="15"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="15"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="15"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="11"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="11"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="11"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="11"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <tabColor rgb="FFFFFFD7"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2249,101 +2791,123 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>119</v>
+      <c r="A1" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="16" t="str">
+      <c r="B2" s="18" t="str">
         <f aca="false">"/path/to/your/project"</f>
         <v>/path/to/your/project</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="16" t="s">
-        <v>120</v>
+      <c r="B3" s="18" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="17" t="s">
-        <v>121</v>
+      <c r="B4" s="19" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="16" t="n">
+      <c r="B5" s="18" t="n">
         <v>44100</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="19" t="n">
+      <c r="B6" s="21"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="21" t="n">
         <v>42000</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="19"/>
-    </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="19" t="s">
-        <v>122</v>
+      <c r="B8" s="21" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="19" t="n">
+      <c r="B9" s="21" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="21" t="n">
         <v>100</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="19" t="n">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="21" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="19" t="n">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="21" t="n">
         <v>40</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="19" t="n">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="21" t="n">
         <v>0.9</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B9" type="list">
+      <formula1>HelpSettings!$A$2:$A$1048576</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" display="http://localhost:3000"/>
   </hyperlinks>
@@ -2357,7 +2921,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFD7"/>
@@ -2375,132 +2939,64 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="20" width="56.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="21" width="42.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="21" width="22.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="22" width="20.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="56.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="23" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="23" width="22.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="24" width="20.56"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1009" min="5" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="23" t="s">
-        <v>123</v>
+      <c r="B1" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="15" t="str">
+      <c r="A2" s="17" t="str">
         <f aca="false">"/path/from/audio/folder"</f>
         <v>/path/from/audio/folder</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>125</v>
+      <c r="B2" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="15"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="15"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="15"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="15"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="16"/>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <tabColor rgb="FFFFFFD7"/>
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B3" activeCellId="0" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="24" width="11.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="25" width="11.84"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="4" style="1" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="23" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="B2" s="25" t="n">
-        <v>20</v>
-      </c>
-      <c r="C2" s="25" t="n">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
+      <c r="C7" s="18"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
feat(Processing/Config): Use ISO 8601 standard
User can now add seconds to file dates and ranges

BREAKING CHANGE: Configuration file now uses ISO 8601 compliant dates
</commit_message>
<xml_diff>
--- a/examples/common/config.xlsx
+++ b/examples/common/config.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="155">
   <si>
     <t xml:space="preserve">Sound Scape Explorer</t>
   </si>
@@ -160,6 +160,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Default</t>
     </r>
@@ -169,6 +170,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> None</t>
     </r>
@@ -206,6 +208,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Default</t>
     </r>
@@ -215,6 +218,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> 15</t>
     </r>
@@ -252,6 +256,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Default</t>
     </r>
@@ -261,6 +266,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> euclidean</t>
     </r>
@@ -298,6 +304,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Default</t>
     </r>
@@ -307,6 +314,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> False</t>
     </r>
@@ -344,6 +352,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Default</t>
     </r>
@@ -353,6 +362,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> 100</t>
     </r>
@@ -390,6 +400,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Default</t>
     </r>
@@ -399,6 +410,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> 20</t>
     </r>
@@ -436,6 +448,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Default</t>
     </r>
@@ -445,6 +458,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> 60</t>
     </r>
@@ -482,6 +496,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Default</t>
     </r>
@@ -491,6 +506,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> 0.9</t>
     </r>
@@ -913,9 +929,6 @@
     <t xml:space="preserve">meta_LABEL</t>
   </si>
   <si>
-    <t xml:space="preserve">20230310 0100</t>
-  </si>
-  <si>
     <t xml:space="preserve">label</t>
   </si>
   <si>
@@ -926,23 +939,18 @@
   </si>
   <si>
     <t xml:space="preserve">r2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20230101 0000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20240101 0000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1001,19 +1009,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <i val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1117,7 +1112,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="34">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1194,7 +1189,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1214,14 +1209,26 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1230,7 +1237,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1727,44 +1738,44 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="11.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="27" width="11.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="29" width="11.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="30" width="11.84"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="4" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="27" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
-        <v>153</v>
-      </c>
-      <c r="B2" s="27" t="n">
+      <c r="A2" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" s="30" t="n">
         <v>20</v>
       </c>
-      <c r="C2" s="27" t="n">
+      <c r="C2" s="30" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1795,35 +1806,35 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="27" width="18.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="29" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="30" width="18.97"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1016" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="27" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
-        <v>154</v>
-      </c>
-      <c r="B2" s="27" t="n">
+      <c r="A2" s="29" t="s">
+        <v>153</v>
+      </c>
+      <c r="B2" s="30" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="24"/>
+      <c r="B4" s="25"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="24"/>
+      <c r="B5" s="25"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="24"/>
+      <c r="B6" s="25"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1854,39 +1865,39 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="27" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="29" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="30" width="20.03"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="4" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="27" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
-        <v>155</v>
-      </c>
-      <c r="B2" s="24" t="s">
-        <v>156</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>157</v>
+      <c r="A2" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2" s="31" t="n">
+        <v>44927</v>
+      </c>
+      <c r="C2" s="31" t="n">
+        <v>45292</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="24"/>
+      <c r="C4" s="25"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1917,47 +1928,47 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="27" width="14.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="27" width="17.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="27" width="15.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="27" width="25.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="29" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="30" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="30" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="30" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="30" width="25.98"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="6" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="32" t="s">
         <v>69</v>
       </c>
       <c r="F1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="B2" s="24" t="n">
+      <c r="B2" s="25" t="n">
         <v>2</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="D2" s="33" t="s">
         <v>153</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="E2" s="33" t="s">
         <v>154</v>
-      </c>
-      <c r="E2" s="29" t="s">
-        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -1999,17 +2010,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="29" width="13.17"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="29" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2052,17 +2063,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="15.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="29" width="15.63"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="29" t="s">
         <v>129</v>
       </c>
     </row>
@@ -2105,27 +2116,27 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="15.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="29" width="15.63"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="29" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="29" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="29" t="s">
         <v>141</v>
       </c>
     </row>
@@ -2164,17 +2175,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="15.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="29" width="15.63"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="29" t="s">
         <v>143</v>
       </c>
     </row>
@@ -2927,7 +2938,7 @@
     <tabColor rgb="FFFFFFD7"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -2941,9 +2952,10 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="56.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="23" width="42.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="23" width="22.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="24" width="20.56"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1009" min="5" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="24" width="22.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="4" style="25" width="20.56"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="34" min="11" style="26" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1009" min="35" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2956,9 +2968,15 @@
       <c r="C1" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="27" t="s">
         <v>150</v>
       </c>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="17" t="str">
@@ -2968,17 +2986,17 @@
       <c r="B2" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="28" t="n">
+        <v>45089.8854166667</v>
+      </c>
+      <c r="D2" s="25" t="s">
         <v>151</v>
-      </c>
-      <c r="D2" s="24" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="17"/>
       <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
+      <c r="C3" s="28"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="17"/>

</xml_diff>

<commit_message>
feat(Processing/Config): Bump version to v10
BREAKING CHANGE: Configuration file has its version bumped to upcoming
v10.
</commit_message>
<xml_diff>
--- a/examples/common/config.xlsx
+++ b/examples/common/config.xlsx
@@ -41,7 +41,7 @@
     <t xml:space="preserve">Sound Scape Explorer</t>
   </si>
   <si>
-    <t xml:space="preserve">Version 9</t>
+    <t xml:space="preserve">Version 10</t>
   </si>
   <si>
     <t xml:space="preserve">Instructions</t>
@@ -1332,7 +1332,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
feat(Processing/Config): Use new `audio_path` setting.
BREAKING CHANGE: Configuration settings `base_path` and `audio_folder`
have been removed and replaced with new merged `audio_path` setting.
</commit_message>
<xml_diff>
--- a/examples/common/config.xlsx
+++ b/examples/common/config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Help" sheetId="1" state="visible" r:id="rId2"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="155">
   <si>
     <t xml:space="preserve">Sound Scape Explorer</t>
   </si>
@@ -917,7 +917,7 @@
     <t xml:space="preserve">value</t>
   </si>
   <si>
-    <t xml:space="preserve">audio</t>
+    <t xml:space="preserve">audio_path</t>
   </si>
   <si>
     <t xml:space="preserve">http://localhost:3000</t>
@@ -945,10 +945,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="General"/>
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -1185,50 +1184,50 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1237,7 +1236,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1329,7 +1328,7 @@
   </sheetPr>
   <dimension ref="A1:B58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B2" activeCellId="0" sqref="B2"/>
@@ -2784,14 +2783,14 @@
     <tabColor rgb="FFFFFFD7"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="bottomRight" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2811,116 +2810,108 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="17" t="s">
-        <v>7</v>
+        <v>147</v>
       </c>
       <c r="B2" s="18" t="str">
-        <f aca="false">"/path/to/your/project"</f>
-        <v>/path/to/your/project</v>
+        <f aca="false">"/path/to/your/audio/folder"</f>
+        <v>/path/to/your/audio/folder</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>147</v>
+        <v>11</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="19" t="s">
-        <v>148</v>
+        <v>12</v>
+      </c>
+      <c r="B4" s="18" t="n">
+        <v>44100</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="18" t="n">
-        <v>44100</v>
-      </c>
+      <c r="A5" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="21"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="B6" s="21" t="n">
+        <v>42000</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="20" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B7" s="21" t="n">
-        <v>42000</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="21" t="n">
-        <v>15</v>
+        <v>20</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="20" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>83</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>149</v>
+        <v>24</v>
+      </c>
+      <c r="B10" s="21" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="20" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B11" s="21" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="20" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B12" s="21" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="20" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B13" s="21" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="21" t="n">
         <v>0.9</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B9" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B8" type="list">
       <formula1>HelpSettings!$A$2:$A$1048576</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" display="http://localhost:3000"/>
+    <hyperlink ref="B3" r:id="rId1" display="http://localhost:3000"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
fix(Config): Change `audio_host` default Docker port
</commit_message>
<xml_diff>
--- a/examples/common/config.xlsx
+++ b/examples/common/config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Help" sheetId="1" state="visible" r:id="rId2"/>
@@ -920,7 +920,7 @@
     <t xml:space="preserve">audio_path</t>
   </si>
   <si>
-    <t xml:space="preserve">http://localhost:3000</t>
+    <t xml:space="preserve">http://localhost:5531</t>
   </si>
   <si>
     <t xml:space="preserve">yes</t>
@@ -945,9 +945,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -1184,7 +1185,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1224,7 +1225,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1236,7 +1237,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1328,10 +1329,10 @@
   </sheetPr>
   <dimension ref="A1:B58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topRight" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1396,8 +1397,8 @@
         <v>11</v>
       </c>
       <c r="B9" s="7" t="str">
-        <f aca="false">"The host name serving your audio files. For Docker, use 'http://localhost:3000'."</f>
-        <v>The host name serving your audio files. For Docker, use 'http://localhost:3000'.</v>
+        <f aca="false">"The host name serving your audio files. For Docker, use 'http://localhost:5531'."</f>
+        <v>The host name serving your audio files. For Docker, use 'http://localhost:5531'.</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2785,12 +2786,12 @@
   </sheetPr>
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2911,7 +2912,7 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="http://localhost:3000"/>
+    <hyperlink ref="B3" r:id="rId1" display="http://localhost:5531"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
feat(Processing/Config): Add `Autoclusters` tab
BREAKING CHANGE: Configuration file has a new `Autoclusters` tab
</commit_message>
<xml_diff>
--- a/examples/common/config.xlsx
+++ b/examples/common/config.xlsx
@@ -5,26 +5,28 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Help" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="HelpSettings" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="HelpReducers" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="HelpIndicators" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="HelpVolumes" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="HelpMatrices" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="HelpPairings" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="Settings" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="Files" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="Bands" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="Integrations" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="Ranges" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="Reducers" sheetId="13" state="visible" r:id="rId14"/>
-    <sheet name="Indicators" sheetId="14" state="visible" r:id="rId15"/>
-    <sheet name="Volumes" sheetId="15" state="visible" r:id="rId16"/>
-    <sheet name="Matrices" sheetId="16" state="visible" r:id="rId17"/>
-    <sheet name="Pairings" sheetId="17" state="visible" r:id="rId18"/>
+    <sheet name="HelpAutoclusters" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="HelpReducers" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="HelpIndicators" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="HelpVolumes" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="HelpMatrices" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="HelpPairings" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Settings" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Files" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Bands" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="Integrations" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="Ranges" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="Autoclusters" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="Reducers" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="Indicators" sheetId="16" state="visible" r:id="rId17"/>
+    <sheet name="Volumes" sheetId="17" state="visible" r:id="rId18"/>
+    <sheet name="Matrices" sheetId="18" state="visible" r:id="rId19"/>
+    <sheet name="Pairings" sheetId="19" state="visible" r:id="rId20"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="161">
   <si>
     <t xml:space="preserve">Sound Scape Explorer</t>
   </si>
@@ -794,6 +796,12 @@
     <t xml:space="preserve">yule</t>
   </si>
   <si>
+    <t xml:space="preserve">hdbscan-eom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hdbscan-leaf</t>
+  </si>
+  <si>
     <t xml:space="preserve">umap</t>
   </si>
   <si>
@@ -939,6 +947,18 @@
   </si>
   <si>
     <t xml:space="preserve">r2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min_cluster_size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min_samples</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alpha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">epsilon</t>
   </si>
 </sst>
 </file>
@@ -1329,7 +1349,7 @@
   </sheetPr>
   <dimension ref="A1:B58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="A2" activeCellId="0" sqref="A2"/>
@@ -1721,6 +1741,101 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <tabColor rgb="FFFFFFD7"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="56.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="23" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="24" width="22.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="4" style="25" width="20.56"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="34" min="11" style="26" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1009" min="35" style="1" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>152</v>
+      </c>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="17" t="str">
+        <f aca="false">"/path/from/audio/folder"</f>
+        <v>/path/from/audio/folder</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="28" t="n">
+        <v>45089.8854166667</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="17"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="28"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="17"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="17"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="17"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="18"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFD7"/>
@@ -1756,7 +1871,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="29" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B2" s="30" t="n">
         <v>20</v>
@@ -1788,7 +1903,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFD7"/>
@@ -1821,7 +1936,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="29" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B2" s="30" t="n">
         <v>15</v>
@@ -1847,7 +1962,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFD7"/>
@@ -1883,7 +1998,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="29" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B2" s="31" t="n">
         <v>44927</v>
@@ -1910,7 +2025,106 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <tabColor rgb="FFFFFFD7"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="29" width="16.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="30" width="16.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="25" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="25" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="25" width="25.98"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="6" style="1" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>160</v>
+      </c>
+      <c r="F1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="25" t="n">
+        <v>15</v>
+      </c>
+      <c r="C2" s="25" t="n">
+        <v>15</v>
+      </c>
+      <c r="D2" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="25" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" s="25" t="n">
+        <v>15</v>
+      </c>
+      <c r="C3" s="25" t="n">
+        <v>15</v>
+      </c>
+      <c r="D3" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="25" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1003" type="list">
+      <formula1>HelpAutoclusters!$A$2:$A$1048576</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1" type="none">
+      <formula1>HelpAutoclusters!$A$2:$A$1048576</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFD7"/>
@@ -1956,19 +2170,19 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="29" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B2" s="25" t="n">
         <v>2</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E2" s="33" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -1992,7 +2206,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFD7"/>
@@ -2021,7 +2235,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="29" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2032,118 +2246,6 @@
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1" type="none">
       <formula1>HelpIndicators!$A$2:$A$1048576</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <tabColor rgb="FFFFFFD7"/>
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="29" width="15.63"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="27" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="29" t="s">
-        <v>129</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1002" type="list">
-      <formula1>HelpVolumes!$A$2:$A$1048576</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1" type="none">
-      <formula1>HelpVolumes!$A$2:$A$1048576</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <tabColor rgb="FFFFFFD7"/>
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:A4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A6" activeCellId="0" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="29" width="15.63"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="27" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="29" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="29" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="29" t="s">
-        <v>141</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1:A1004" type="list">
-      <formula1>HelpMatrices!$A$2:$A$1048576</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -2170,6 +2272,118 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="29" width="15.63"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="29" t="s">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1002" type="list">
+      <formula1>HelpVolumes!$A$2:$A$1048576</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1" type="none">
+      <formula1>HelpVolumes!$A$2:$A$1048576</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <tabColor rgb="FFFFFFD7"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A6" activeCellId="0" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="29" width="15.63"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="27" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="29" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="29" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="29" t="s">
+        <v>143</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1:A1004" type="list">
+      <formula1>HelpMatrices!$A$2:$A$1048576</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <tabColor rgb="FFFFFFD7"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2186,7 +2400,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="29" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -2365,6 +2579,54 @@
     <tabColor rgb="FFEEEEEE"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="16.24"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="2" style="1" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <tabColor rgb="FFEEEEEE"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -2388,136 +2650,22 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="12" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <tabColor rgb="FFEEEEEE"/>
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B10"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="42.79"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
         <v>111</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -2556,58 +2704,83 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="12" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="12" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="15"/>
+      <c r="A6" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="11"/>
+      <c r="A7" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="11"/>
+      <c r="A8" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="11"/>
+      <c r="A9" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="11"/>
+      <c r="A10" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>130</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2621,6 +2794,95 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <tabColor rgb="FFEEEEEE"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="42.79"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="15"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="11"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="11"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="11"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="11"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFEEEEEE"/>
@@ -2648,31 +2910,31 @@
         <v>78</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="12" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2704,7 +2966,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFEEEEEE"/>
@@ -2732,15 +2994,15 @@
         <v>78</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2778,7 +3040,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFD7"/>
@@ -2803,15 +3065,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="16" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="17" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B2" s="18" t="str">
         <f aca="false">"/path/to/your/audio/folder"</f>
@@ -2823,7 +3085,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2869,7 +3131,7 @@
         <v>22</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2922,99 +3184,4 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <tabColor rgb="FFFFFFD7"/>
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:J7"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="56.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="23" width="42.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="24" width="22.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="4" style="25" width="20.56"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="34" min="11" style="26" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1009" min="35" style="1" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="27" t="s">
-        <v>150</v>
-      </c>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="17" t="str">
-        <f aca="false">"/path/from/audio/folder"</f>
-        <v>/path/from/audio/folder</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="28" t="n">
-        <v>45089.8854166667</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="17"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="28"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="17"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="17"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="17"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="18"/>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
feat(Processing/Config): Add new computation UMAP settings + Remove unneeded settings
BREAKING CHANGE: The configuration file has new settings and some old
settings have been removed.
</commit_message>
<xml_diff>
--- a/examples/common/config.xlsx
+++ b/examples/common/config.xlsx
@@ -5,28 +5,27 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="13"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Help" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="HelpSettings" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="HelpAutoclusters" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="HelpReducers" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="HelpIndicators" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="HelpVolumes" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="HelpMatrices" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="HelpPairings" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="Settings" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="Files" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="Bands" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="Integrations" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="Ranges" sheetId="13" state="visible" r:id="rId14"/>
-    <sheet name="Autoclusters" sheetId="14" state="visible" r:id="rId15"/>
-    <sheet name="Reducers" sheetId="15" state="visible" r:id="rId16"/>
-    <sheet name="Indicators" sheetId="16" state="visible" r:id="rId17"/>
-    <sheet name="Volumes" sheetId="17" state="visible" r:id="rId18"/>
-    <sheet name="Matrices" sheetId="18" state="visible" r:id="rId19"/>
-    <sheet name="Pairings" sheetId="19" state="visible" r:id="rId20"/>
+    <sheet name="HelpAutoclusters" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="HelpReducers" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="HelpIndicators" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="HelpVolumes" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="HelpMatrices" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="HelpPairings" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Settings" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Files" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Bands" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Integrations" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="Ranges" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="Autoclusters" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="Reducers" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="Indicators" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="Volumes" sheetId="16" state="visible" r:id="rId17"/>
+    <sheet name="Matrices" sheetId="17" state="visible" r:id="rId18"/>
+    <sheet name="Pairings" sheetId="18" state="visible" r:id="rId19"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="128">
   <si>
     <t xml:space="preserve">Sound Scape Explorer</t>
   </si>
@@ -85,17 +84,6 @@
     <t xml:space="preserve">timezone</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Optional</t>
-    </r>
     <r>
       <rPr>
         <i val="true"/>
@@ -104,8 +92,18 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> The timezone of your project. If empty, dates and times will display as UTC.
+      <t xml:space="preserve">The timezone of your project. If empty, dates and times will display as UTC.
 </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Optional, </t>
     </r>
     <r>
       <rPr>
@@ -130,20 +128,9 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">umap_seed</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Optional </t>
-    </r>
+    <t xml:space="preserve">computation_umap_iterations</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <i val="true"/>
@@ -152,8 +139,18 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">The seed number used for UMAP reductions. Also used for PCA based reductions.
+      <t xml:space="preserve">The number of UMAPs generated for computation purposes.
 </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Optional, </t>
     </r>
     <r>
       <rPr>
@@ -178,20 +175,9 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">umap_neighbors</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Optional </t>
-    </r>
+    <t xml:space="preserve">computation_umap_dimensions</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <i val="true"/>
@@ -200,8 +186,18 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">The size of local neighborhood used for UMAP.
+      <t xml:space="preserve">The dimensions of UMAPs generated for computation purposes.
 </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Optional, </t>
     </r>
     <r>
       <rPr>
@@ -222,24 +218,13 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> 15</t>
+      <t xml:space="preserve"> None</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">umap_metric</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Optional </t>
-    </r>
+    <t xml:space="preserve">display_umap_seed</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <i val="true"/>
@@ -248,8 +233,18 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">The metric to use to compute distances in high dimensional space.
+      <t xml:space="preserve">The randomness seed used for display UMAPs. Also used for PCAs.
 </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Optional, </t>
     </r>
     <r>
       <rPr>
@@ -270,247 +265,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> euclidean</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">autocluster</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Optional</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Whether you want to run auto clustering process. `yes` or `no`.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Default</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> False</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">autocluster_iterations</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Optional</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> The number of iterations during the autoclustering process.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Default</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> 100</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">autocluster_min_size</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Optional</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> The minimum expected size of clusters.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Default</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> 20</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">autocluster_max_size</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Optional</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> The maximum expected size of clusters.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Default</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> 60</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">autocluster_threshold</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Optional</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> The threshold to specify membership of given element in a cluster.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Default</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> 0.9</t>
+      <t xml:space="preserve"> None</t>
     </r>
   </si>
   <si>
@@ -727,73 +482,7 @@
     <t xml:space="preserve">The pairing. See `HelpPairings` tab for available options.</t>
   </si>
   <si>
-    <t xml:space="preserve">euclidean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">manhattan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chebyshev</t>
-  </si>
-  <si>
-    <t xml:space="preserve">minkowski</t>
-  </si>
-  <si>
-    <t xml:space="preserve">canberra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">braycurtis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mahalanobis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wminkowski</t>
-  </si>
-  <si>
-    <t xml:space="preserve">seuclidean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cosine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">correlation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">haversine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hamming</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jaccard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">russelrao</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kulsinski</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ll_dirichlet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hellinger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rogerstanimoto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sokalmichener</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sokalsneath</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yule</t>
+    <t xml:space="preserve">autocluster</t>
   </si>
   <si>
     <t xml:space="preserve">hdbscan-eom</t>
@@ -929,9 +618,6 @@
   </si>
   <si>
     <t xml:space="preserve">http://localhost:5531</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes</t>
   </si>
   <si>
     <t xml:space="preserve">meta_LABEL</t>
@@ -970,7 +656,7 @@
     <numFmt numFmtId="165" formatCode="General"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1029,6 +715,13 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <i val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1132,7 +825,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1169,14 +862,18 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1209,7 +906,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1261,7 +958,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1347,17 +1044,17 @@
     <tabColor rgb="FFEEEEEE"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B58"/>
+  <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topRight" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="29.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="90.96"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="3" style="1" width="11.52"/>
   </cols>
@@ -1429,7 +1126,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
         <v>14</v>
       </c>
@@ -1437,7 +1134,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
         <v>16</v>
       </c>
@@ -1445,7 +1142,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
         <v>18</v>
       </c>
@@ -1453,7 +1150,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
         <v>20</v>
       </c>
@@ -1461,266 +1158,226 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8" t="s">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="9" t="s">
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="9" t="s">
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8" t="s">
+      <c r="B19" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="9" t="s">
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="8" t="s">
+      <c r="B20" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="9" t="s">
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="2"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>34</v>
-      </c>
+      <c r="B22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="2"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B32" s="7" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B32" s="2"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B36" s="2"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B38" s="7" t="s">
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="10" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="6" t="s">
+      <c r="B40" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B39" s="7" t="s">
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="10" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="2" t="s">
+      <c r="B41" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="B41" s="2"/>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="6" t="s">
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B43" s="2"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="6" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="6" t="s">
+      <c r="B44" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="B43" s="7" t="s">
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="10" t="s">
+      <c r="B46" s="2"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B44" s="9" t="s">
+      <c r="B47" s="12" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="10" t="s">
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B45" s="9" t="s">
+      <c r="B49" s="2"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="6" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="10" t="s">
+      <c r="B50" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B46" s="9" t="s">
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="2" t="s">
+      <c r="B52" s="2"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B48" s="2"/>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="6" t="s">
+      <c r="B53" s="12" t="s">
         <v>72</v>
-      </c>
-      <c r="B49" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B51" s="2"/>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B52" s="11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B54" s="2"/>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B55" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B57" s="2"/>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B58" s="11" t="s">
-        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1746,83 +1403,56 @@
     <tabColor rgb="FFFFFFD7"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="56.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="23" width="42.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="24" width="22.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="4" style="25" width="20.56"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="34" min="11" style="26" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1009" min="35" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="11.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="31" width="11.84"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="4" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="27" t="s">
-        <v>152</v>
-      </c>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
+      <c r="A1" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="17" t="str">
-        <f aca="false">"/path/from/audio/folder"</f>
-        <v>/path/from/audio/folder</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="28" t="n">
-        <v>45089.8854166667</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="17"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="28"/>
+      <c r="A2" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" s="31" t="n">
+        <v>20</v>
+      </c>
+      <c r="C2" s="31" t="n">
+        <v>20000</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="17"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="17"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="17"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="18"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1841,56 +1471,47 @@
     <tabColor rgb="FFFFFFD7"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="29" width="11.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="30" width="11.84"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="4" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="31" width="18.97"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1016" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" s="27" t="s">
-        <v>46</v>
+      <c r="A1" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="29" t="s">
-        <v>154</v>
-      </c>
-      <c r="B2" s="30" t="n">
-        <v>20</v>
-      </c>
-      <c r="C2" s="30" t="n">
-        <v>20000</v>
+      <c r="A2" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="31" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
+      <c r="B4" s="26"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
+      <c r="B5" s="26"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
+      <c r="B6" s="26"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1909,7 +1530,7 @@
     <tabColor rgb="FFFFFFD7"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -1921,35 +1542,39 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="29" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="30" width="18.97"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1016" min="3" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="31" width="20.03"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="4" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" s="27" t="s">
-        <v>51</v>
+      <c r="A1" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="29" t="s">
-        <v>155</v>
-      </c>
-      <c r="B2" s="30" t="n">
-        <v>15</v>
-      </c>
+      <c r="A2" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="32" t="n">
+        <v>44927</v>
+      </c>
+      <c r="C2" s="32" t="n">
+        <v>45292</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="25"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="25"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="25"/>
+      <c r="C4" s="26"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1968,7 +1593,7 @@
     <tabColor rgb="FFFFFFD7"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -1980,41 +1605,60 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="29" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="30" width="20.03"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="4" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="16.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="31" width="16.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="26" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="26" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="26" width="25.98"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="6" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" s="27" t="s">
-        <v>58</v>
-      </c>
+      <c r="A1" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="29" t="s">
-        <v>156</v>
-      </c>
-      <c r="B2" s="31" t="n">
-        <v>44927</v>
-      </c>
-      <c r="C2" s="31" t="n">
-        <v>45292</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="25"/>
+      <c r="A2" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="26" t="n">
+        <v>15</v>
+      </c>
+      <c r="C2" s="26" t="n">
+        <v>15</v>
+      </c>
+      <c r="D2" s="26" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="26" t="n">
+        <v>0.1</v>
+      </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1002" type="list">
+      <formula1>HelpAutoclusters!$A$2:$A$1048576</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1" type="none">
+      <formula1>HelpAutoclusters!$A$2:$A$1048576</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2031,86 +1675,69 @@
     <tabColor rgb="FFFFFFD7"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="29" width="16.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="30" width="16.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="25" width="17.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="25" width="15.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="25" width="25.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="31" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="31" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="31" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="31" width="25.98"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="6" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="27" t="s">
-        <v>157</v>
-      </c>
-      <c r="C1" s="27" t="s">
-        <v>158</v>
-      </c>
-      <c r="D1" s="27" t="s">
-        <v>159</v>
-      </c>
-      <c r="E1" s="27" t="s">
-        <v>160</v>
+      <c r="A1" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>59</v>
       </c>
       <c r="F1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="B2" s="25" t="n">
-        <v>15</v>
-      </c>
-      <c r="C2" s="25" t="n">
-        <v>15</v>
-      </c>
-      <c r="D2" s="25" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" s="25" t="n">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="29" t="s">
-        <v>107</v>
-      </c>
-      <c r="B3" s="25" t="n">
-        <v>15</v>
-      </c>
-      <c r="C3" s="25" t="n">
-        <v>15</v>
-      </c>
-      <c r="D3" s="25" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" s="25" t="n">
-        <v>0.1</v>
+      <c r="A2" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="26" t="n">
+        <v>3</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1003" type="list">
-      <formula1>HelpAutoclusters!$A$2:$A$1048576</formula1>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1002" type="list">
+      <formula1>HelpReducers!$A$2:$A$1048576</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1" type="none">
-      <formula1>HelpAutoclusters!$A$2:$A$1048576</formula1>
+      <formula1>HelpReducers!$A$2:$A$1048576</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -2130,69 +1757,40 @@
     <tabColor rgb="FFFFFFD7"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="29" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="30" width="14.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="30" width="17.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="30" width="15.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="30" width="25.98"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="6" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="13.17"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="C1" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="D1" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="E1" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="F1" s="0"/>
+      <c r="A1" s="28" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="29" t="s">
-        <v>108</v>
-      </c>
-      <c r="B2" s="25" t="n">
-        <v>2</v>
-      </c>
-      <c r="C2" s="33" t="s">
-        <v>154</v>
-      </c>
-      <c r="D2" s="33" t="s">
-        <v>155</v>
-      </c>
-      <c r="E2" s="33" t="s">
-        <v>156</v>
+      <c r="A2" s="30" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1002" type="list">
-      <formula1>HelpReducers!$A$2:$A$1048576</formula1>
+      <formula1>HelpIndicators!$A$2:$A$1048576</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1" type="none">
-      <formula1>HelpReducers!$A$2:$A$1048576</formula1>
+      <formula1>HelpIndicators!$A$2:$A$1048576</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -2219,33 +1817,33 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="29" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="15.63"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="27" t="s">
-        <v>72</v>
+      <c r="A1" s="28" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="29" t="s">
-        <v>129</v>
+      <c r="A2" s="30" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1002" type="list">
-      <formula1>HelpIndicators!$A$2:$A$1048576</formula1>
+      <formula1>HelpVolumes!$A$2:$A$1048576</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1" type="none">
-      <formula1>HelpIndicators!$A$2:$A$1048576</formula1>
+      <formula1>HelpVolumes!$A$2:$A$1048576</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -2272,33 +1870,29 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="29" width="15.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="15.63"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="27" t="s">
-        <v>75</v>
+      <c r="A1" s="28" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="29" t="s">
-        <v>131</v>
+      <c r="A2" s="30" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1002" type="list">
-      <formula1>HelpVolumes!$A$2:$A$1048576</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1" type="none">
-      <formula1>HelpVolumes!$A$2:$A$1048576</formula1>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1:A1002" type="list">
+      <formula1>HelpMatrices!$A$2:$A$1048576</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -2318,65 +1912,6 @@
     <tabColor rgb="FFFFFFD7"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A6" activeCellId="0" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="29" width="15.63"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="27" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="29" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="29" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="29" t="s">
-        <v>143</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1:A1004" type="list">
-      <formula1>HelpMatrices!$A$2:$A$1048576</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <tabColor rgb="FFFFFFD7"/>
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -2384,23 +1919,23 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="29" width="15.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="15.63"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="27" t="s">
-        <v>81</v>
+      <c r="A1" s="28" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="29" t="s">
-        <v>145</v>
+      <c r="A2" s="30" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -2426,140 +1961,35 @@
     <tabColor rgb="FFEEEEEE"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A24"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="16.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="16.24"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
-        <v>20</v>
+      <c r="A1" s="14" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
-        <v>83</v>
+      <c r="A2" s="13" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="12" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="12" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="12" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="12" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="12" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="12" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="12" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="12" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="12" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="12" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="12" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="12" t="s">
-        <v>105</v>
+      <c r="A3" s="13" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -2579,35 +2009,45 @@
     <tabColor rgb="FFEEEEEE"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="16.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="16.24"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
-        <v>22</v>
+      <c r="A1" s="14" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
-        <v>106</v>
+      <c r="A2" s="13" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="s">
-        <v>107</v>
+      <c r="A3" s="13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="13" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -2627,7 +2067,7 @@
     <tabColor rgb="FFEEEEEE"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -2639,33 +2079,89 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="16.24"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="2" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="15" width="42.79"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
-        <v>61</v>
+      <c r="A1" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
-        <v>108</v>
+      <c r="A2" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="s">
-        <v>109</v>
+      <c r="A3" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
-        <v>110</v>
+      <c r="A4" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12" t="s">
-        <v>111</v>
+      <c r="A5" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -2697,90 +2193,65 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="15" width="42.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
-        <v>72</v>
+      <c r="A1" s="14" t="s">
+        <v>65</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>112</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>114</v>
+      <c r="A2" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>116</v>
+      <c r="A3" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>118</v>
+      <c r="A4" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>120</v>
+      <c r="A5" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>122</v>
-      </c>
+      <c r="B6" s="16"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>124</v>
-      </c>
+      <c r="B7" s="12"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>126</v>
-      </c>
+      <c r="B8" s="12"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>128</v>
-      </c>
+      <c r="B9" s="12"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>130</v>
-      </c>
+      <c r="B10" s="12"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2806,70 +2277,65 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="15" width="42.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
-        <v>75</v>
+      <c r="A1" s="14" t="s">
+        <v>68</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>136</v>
-      </c>
-    </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>138</v>
-      </c>
+      <c r="B5" s="16"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="15"/>
+      <c r="B6" s="16"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="11"/>
+      <c r="B7" s="12"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="11"/>
+      <c r="B8" s="12"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="11"/>
+      <c r="B9" s="12"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="11"/>
+      <c r="B10" s="12"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2895,65 +2361,55 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="15" width="42.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
-        <v>78</v>
+      <c r="A1" s="14" t="s">
+        <v>68</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>112</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>140</v>
+      <c r="A2" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>142</v>
-      </c>
+      <c r="B3" s="16"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>144</v>
-      </c>
+      <c r="B4" s="16"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="15"/>
+      <c r="B5" s="16"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="15"/>
+      <c r="B6" s="16"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="11"/>
+      <c r="B7" s="12"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="11"/>
+      <c r="B8" s="12"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="11"/>
+      <c r="B9" s="12"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="11"/>
+      <c r="B10" s="12"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2969,67 +2425,93 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
-    <tabColor rgb="FFEEEEEE"/>
+    <tabColor rgb="FFFFFFD7"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="42.79"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="29.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.24"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>112</v>
+      <c r="A1" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>146</v>
+      <c r="A2" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="19" t="str">
+        <f aca="false">"/path/to/your/audio/folder"</f>
+        <v>/path/to/your/audio/folder</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="15"/>
+      <c r="A3" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="15"/>
+      <c r="A4" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="19" t="n">
+        <v>44100</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="15"/>
+      <c r="A5" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="22"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="15"/>
+      <c r="A6" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="22" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="11"/>
+      <c r="A7" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="22" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="11"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="11"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="11"/>
+      <c r="A8" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="22" t="n">
+        <v>42000</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" display="http://localhost:5531"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3046,136 +2528,85 @@
     <tabColor rgb="FFFFFFD7"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.24"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="3" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="56.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="24" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="25" width="22.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="4" style="26" width="20.56"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="34" min="11" style="27" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1009" min="35" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>148</v>
-      </c>
+      <c r="A1" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="B2" s="18" t="str">
-        <f aca="false">"/path/to/your/audio/folder"</f>
-        <v>/path/to/your/audio/folder</v>
+      <c r="A2" s="18" t="str">
+        <f aca="false">"/path/from/audio/folder"</f>
+        <v>/path/from/audio/folder</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="29" t="n">
+        <v>45089.8854166667</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="19" t="s">
-        <v>150</v>
-      </c>
+      <c r="A3" s="18"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="29"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="18" t="n">
-        <v>44100</v>
-      </c>
+      <c r="A4" s="18"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="21"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="21" t="n">
-        <v>42000</v>
-      </c>
+      <c r="A6" s="18"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="21" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="21" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="21" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="21" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="21" t="n">
-        <v>0.9</v>
-      </c>
+      <c r="C7" s="19"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B8" type="list">
-      <formula1>HelpSettings!$A$2:$A$1048576</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="http://localhost:5531"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
feat(Processing/Config): Digest new settings + Improve documentation (Help tab)
</commit_message>
<xml_diff>
--- a/examples/common/config.xlsx
+++ b/examples/common/config.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="126">
   <si>
     <t xml:space="preserve">Sound Scape Explorer</t>
   </si>
@@ -60,25 +60,51 @@
     <t xml:space="preserve">Settings</t>
   </si>
   <si>
-    <t xml:space="preserve">base_path</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The relative or absolute path to your project folder. Examples: `./relative/project` `/absolute/project`.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">audio_folder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The name of the folder containing your audio samples.</t>
+    <t xml:space="preserve">audio_path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The relative or absolute path to your audio folder.
+Examples: `./relative/path/to/audio` `/absolute/path/to/audio`.</t>
   </si>
   <si>
     <t xml:space="preserve">audio_host</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">The host name serving your audio files.
+For Docker, use '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">http://localhost:5531</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">'.</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">expected_sample_rate</t>
   </si>
   <si>
-    <t xml:space="preserve">The sample rate of your audio samples.</t>
+    <t xml:space="preserve">The sample rate of your audio samples in Hertz.</t>
   </si>
   <si>
     <t xml:space="preserve">timezone</t>
@@ -102,8 +128,35 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Optional, </t>
+      <t xml:space="preserve">Optional, Default</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> None</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">computation_umap_dimensions</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">The dimensions of UMAPs generated for computation purposes.
+</t>
     </r>
     <r>
       <rPr>
@@ -114,7 +167,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Default</t>
+      <t xml:space="preserve">Optional, Default</t>
     </r>
     <r>
       <rPr>
@@ -124,7 +177,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> None</t>
+      <t xml:space="preserve"> 5</t>
     </r>
   </si>
   <si>
@@ -149,19 +202,9 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Optional, </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Default</t>
+      <t xml:space="preserve">Optional, Default</t>
     </r>
     <r>
       <rPr>
@@ -171,54 +214,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> None</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">computation_umap_dimensions</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">The dimensions of UMAPs generated for computation purposes.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Optional, </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Default</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> None</t>
+      <t xml:space="preserve"> 50</t>
     </r>
   </si>
   <si>
@@ -243,19 +239,9 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Optional, </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Default</t>
+      <t xml:space="preserve">Optional, Default</t>
     </r>
     <r>
       <rPr>
@@ -265,7 +251,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> None</t>
+      <t xml:space="preserve"> 42000</t>
     </r>
   </si>
   <si>
@@ -614,9 +600,6 @@
     <t xml:space="preserve">value</t>
   </si>
   <si>
-    <t xml:space="preserve">audio_path</t>
-  </si>
-  <si>
     <t xml:space="preserve">http://localhost:5531</t>
   </si>
   <si>
@@ -656,7 +639,7 @@
     <numFmt numFmtId="165" formatCode="General"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -702,6 +685,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <i val="true"/>
       <sz val="10"/>
@@ -712,20 +702,6 @@
     <font>
       <i val="true"/>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <i val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -825,7 +801,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -851,30 +827,38 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -890,7 +874,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -906,15 +890,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -958,11 +942,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1044,12 +1028,12 @@
     <tabColor rgb="FFEEEEEE"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B53"/>
+  <dimension ref="A1:B52"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topRight" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1093,7 +1077,7 @@
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
         <v>7</v>
       </c>
@@ -1101,7 +1085,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
         <v>9</v>
       </c>
@@ -1110,274 +1094,265 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="7" t="str">
-        <f aca="false">"The host name serving your audio files. For Docker, use 'http://localhost:5531'."</f>
-        <v>The host name serving your audio files. For Docker, use 'http://localhost:5531'.</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
+      <c r="B9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="7" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="10" t="s">
         <v>13</v>
       </c>
+      <c r="B10" s="11" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="9" t="s">
+      <c r="A11" s="10" t="s">
         <v>15</v>
       </c>
+      <c r="B11" s="11" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="9" t="s">
+      <c r="A12" s="10" t="s">
         <v>17</v>
       </c>
+      <c r="B12" s="11" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="9" t="s">
+      <c r="A13" s="10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8" t="s">
+      <c r="B13" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="9" t="s">
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="B15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B16" s="7" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6" t="s">
-        <v>23</v>
+      <c r="A17" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="6" t="s">
-        <v>25</v>
+      <c r="A18" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6" t="s">
-        <v>27</v>
+      <c r="A19" s="8" t="s">
+        <v>28</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="7" t="s">
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="B21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="2"/>
+      <c r="B22" s="7" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6" t="s">
-        <v>32</v>
+      <c r="A23" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6" t="s">
-        <v>34</v>
+      <c r="A24" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="7" t="s">
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="B26" s="2"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="2"/>
+      <c r="B27" s="7" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="6" t="s">
-        <v>39</v>
+      <c r="A28" s="8" t="s">
+        <v>40</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B29" s="7" t="s">
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="B30" s="2"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="2"/>
+      <c r="B31" s="7" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="6" t="s">
-        <v>44</v>
+      <c r="A32" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="6" t="s">
-        <v>46</v>
+      <c r="A33" s="8" t="s">
+        <v>47</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B34" s="7" t="s">
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2" t="s">
         <v>49</v>
       </c>
+      <c r="B35" s="2"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B36" s="2"/>
+      <c r="B36" s="7" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="6" t="s">
-        <v>51</v>
+      <c r="A37" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B38" s="7" t="s">
+      <c r="A38" s="12" t="s">
         <v>54</v>
       </c>
+      <c r="B38" s="13" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="B39" s="11" t="s">
+      <c r="A39" s="12" t="s">
         <v>56</v>
       </c>
+      <c r="B39" s="13" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B40" s="11" t="s">
+      <c r="A40" s="12" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="10" t="s">
+      <c r="B40" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B41" s="11" t="s">
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="2" t="s">
         <v>60</v>
       </c>
+      <c r="B42" s="2"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B43" s="2"/>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="6" t="s">
+      <c r="B43" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="B44" s="12" t="s">
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="B45" s="2"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="B46" s="2"/>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="6" t="s">
+      <c r="B46" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="B47" s="12" t="s">
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="2" t="s">
         <v>66</v>
       </c>
+      <c r="B48" s="2"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B49" s="2"/>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="6" t="s">
+      <c r="B49" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="B50" s="12" t="s">
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="2" t="s">
         <v>69</v>
       </c>
+      <c r="B51" s="2"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B52" s="2"/>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="6" t="s">
+      <c r="B52" s="14" t="s">
         <v>71</v>
-      </c>
-      <c r="B53" s="12" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1386,6 +1361,7 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" location="readme" display="Find documentation here: https://github.com/sound-scape-explorer/sound-scape-explorer#readme"/>
+    <hyperlink ref="B8" r:id="rId2" display="http://localhost:5531"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1415,44 +1391,44 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="11.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="31" width="11.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="32" width="11.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="33" width="11.84"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="4" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="28" t="s">
-        <v>36</v>
+      <c r="A1" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="B2" s="31" t="n">
+      <c r="A2" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="33" t="n">
         <v>20</v>
       </c>
-      <c r="C2" s="31" t="n">
+      <c r="C2" s="33" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1483,35 +1459,35 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="31" width="18.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="32" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="33" width="18.97"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1016" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="28" t="s">
-        <v>41</v>
+      <c r="A1" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30" t="s">
-        <v>122</v>
-      </c>
-      <c r="B2" s="31" t="n">
+      <c r="A2" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" s="33" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="26"/>
+      <c r="B4" s="28"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="26"/>
+      <c r="B5" s="28"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="26"/>
+      <c r="B6" s="28"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1542,39 +1518,39 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="31" width="20.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="32" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="33" width="20.03"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="4" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="28" t="s">
-        <v>48</v>
+      <c r="A1" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30" t="s">
-        <v>123</v>
-      </c>
-      <c r="B2" s="32" t="n">
+      <c r="A2" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" s="34" t="n">
         <v>44927</v>
       </c>
-      <c r="C2" s="32" t="n">
+      <c r="C2" s="34" t="n">
         <v>45292</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="26"/>
+      <c r="C4" s="28"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1605,46 +1581,46 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="16.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="31" width="16.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="26" width="17.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="26" width="15.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="26" width="25.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="32" width="16.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="33" width="16.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="28" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="28" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="28" width="25.98"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="6" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="F1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="28" t="s">
-        <v>124</v>
-      </c>
-      <c r="C1" s="28" t="s">
-        <v>125</v>
-      </c>
-      <c r="D1" s="28" t="s">
-        <v>126</v>
-      </c>
-      <c r="E1" s="28" t="s">
-        <v>127</v>
-      </c>
-      <c r="F1" s="0"/>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" s="26" t="n">
+      <c r="B2" s="28" t="n">
         <v>15</v>
       </c>
-      <c r="C2" s="26" t="n">
+      <c r="C2" s="28" t="n">
         <v>15</v>
       </c>
-      <c r="D2" s="26" t="n">
+      <c r="D2" s="28" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="26" t="n">
+      <c r="E2" s="28" t="n">
         <v>0.1</v>
       </c>
     </row>
@@ -1687,47 +1663,47 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="31" width="14.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="31" width="17.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="31" width="15.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="31" width="25.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="32" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="33" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="33" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="33" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="33" width="25.98"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="6" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="C1" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="E1" s="33" t="s">
-        <v>59</v>
+      <c r="A1" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="35" t="s">
+        <v>58</v>
       </c>
       <c r="F1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="B2" s="26" t="n">
+      <c r="A2" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="28" t="n">
         <v>3</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="36" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="E2" s="36" t="s">
         <v>121</v>
-      </c>
-      <c r="D2" s="34" t="s">
-        <v>122</v>
-      </c>
-      <c r="E2" s="34" t="s">
-        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1769,18 +1745,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="32" width="13.17"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28" t="s">
-        <v>62</v>
+      <c r="A1" s="30" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30" t="s">
-        <v>97</v>
+      <c r="A2" s="32" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1822,18 +1798,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="15.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="32" width="15.63"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28" t="s">
-        <v>65</v>
+      <c r="A1" s="30" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30" t="s">
-        <v>99</v>
+      <c r="A2" s="32" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1875,18 +1851,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="15.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="32" width="15.63"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28" t="s">
-        <v>68</v>
+      <c r="A1" s="30" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30" t="s">
-        <v>111</v>
+      <c r="A2" s="32" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1924,18 +1900,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="15.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="32" width="15.63"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28" t="s">
-        <v>71</v>
+      <c r="A1" s="30" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30" t="s">
-        <v>113</v>
+      <c r="A2" s="32" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1973,23 +1949,23 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="16.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="15" width="16.24"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="15" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="15" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -2021,33 +1997,33 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="16.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="15" width="16.24"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="14" t="s">
-        <v>51</v>
+      <c r="A1" s="16" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="15" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13" t="s">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="15" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="13" t="s">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="15" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -2079,89 +2055,89 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="15" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="15" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="42.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="14" t="s">
-        <v>62</v>
+      <c r="A1" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="15" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="s">
+      <c r="B2" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="16" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="15" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13" t="s">
+      <c r="B3" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="B3" s="16" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="15" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="13" t="s">
+      <c r="B4" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="16" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="15" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13" t="s">
+      <c r="B5" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="B5" s="16" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="15" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="13" t="s">
+      <c r="B6" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="B6" s="16" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="15" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="13" t="s">
+      <c r="B7" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="B7" s="12" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="15" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="13" t="s">
+      <c r="B8" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="B8" s="12" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="15" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="13" t="s">
+      <c r="B9" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="B9" s="12" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="15" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="13" t="s">
+      <c r="B10" s="14" t="s">
         <v>97</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -2193,65 +2169,65 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="15" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="15" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="42.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="14" t="s">
-        <v>65</v>
+      <c r="A1" s="16" t="s">
+        <v>64</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="16" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="15" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13" t="s">
+      <c r="B3" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="B3" s="16" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="15" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="13" t="s">
+      <c r="B4" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="B4" s="16" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="15" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13" t="s">
+      <c r="B5" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>106</v>
-      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="16"/>
+      <c r="B6" s="18"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="12"/>
+      <c r="B7" s="14"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="12"/>
+      <c r="B8" s="14"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="12"/>
+      <c r="B9" s="14"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="12"/>
+      <c r="B10" s="14"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2282,60 +2258,60 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="15" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="15" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="42.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="14" t="s">
-        <v>68</v>
+      <c r="A1" s="16" t="s">
+        <v>67</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="B2" s="16" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="15" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13" t="s">
+      <c r="B3" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="B3" s="16" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="15" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="13" t="s">
+      <c r="B4" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>112</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="16"/>
+      <c r="B5" s="18"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="16"/>
+      <c r="B6" s="18"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="12"/>
+      <c r="B7" s="14"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="12"/>
+      <c r="B8" s="14"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="12"/>
+      <c r="B9" s="14"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="12"/>
+      <c r="B10" s="14"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2366,50 +2342,50 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="15" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="15" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="42.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="14" t="s">
-        <v>68</v>
+      <c r="A1" s="16" t="s">
+        <v>67</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>114</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="16"/>
+      <c r="B3" s="18"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="16"/>
+      <c r="B4" s="18"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="16"/>
+      <c r="B5" s="18"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="16"/>
+      <c r="B6" s="18"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="12"/>
+      <c r="B7" s="14"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="12"/>
+      <c r="B8" s="14"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="12"/>
+      <c r="B9" s="14"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="12"/>
+      <c r="B10" s="14"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2435,7 +2411,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2446,65 +2422,65 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="17" t="s">
-        <v>116</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="B2" s="19" t="str">
+      <c r="A2" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="21" t="str">
         <f aca="false">"/path/to/your/audio/folder"</f>
         <v>/path/to/your/audio/folder</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="20" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="19" t="n">
+      <c r="B4" s="21" t="n">
         <v>44100</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="22"/>
+      <c r="A5" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="24"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="22" t="n">
+      <c r="A6" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="24" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="22" t="n">
+      <c r="A7" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="24" t="n">
         <v>50</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="22" t="n">
+      <c r="A8" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="24" t="n">
         <v>42000</v>
       </c>
     </row>
@@ -2540,71 +2516,71 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="56.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="24" width="42.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="25" width="22.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="4" style="26" width="20.56"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="34" min="11" style="27" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="25" width="56.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="26" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="27" width="22.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="4" style="28" width="20.56"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="34" min="11" style="29" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1009" min="35" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="28" t="s">
-        <v>119</v>
-      </c>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="A1" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="18" t="str">
+      <c r="A2" s="20" t="str">
         <f aca="false">"/path/from/audio/folder"</f>
         <v>/path/from/audio/folder</v>
       </c>
-      <c r="B2" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="29" t="n">
+      <c r="B2" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="31" t="n">
         <v>45089.8854166667</v>
       </c>
-      <c r="D2" s="26" t="s">
-        <v>120</v>
+      <c r="D2" s="28" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="18"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="29"/>
+      <c r="A3" s="20"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="31"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="18"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
+      <c r="A4" s="20"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="18"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
+      <c r="A5" s="20"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="18"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
+      <c r="A6" s="20"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="19"/>
+      <c r="C7" s="21"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
feat(Config): Add new `Trajectories` tab
BREAKING CHANGE: Excel configuration file has a new tab.
</commit_message>
<xml_diff>
--- a/examples/common/config.xlsx
+++ b/examples/common/config.xlsx
@@ -21,11 +21,12 @@
     <sheet name="Integrations" sheetId="11" state="visible" r:id="rId12"/>
     <sheet name="Ranges" sheetId="12" state="visible" r:id="rId13"/>
     <sheet name="Autoclusters" sheetId="13" state="visible" r:id="rId14"/>
-    <sheet name="Reducers" sheetId="14" state="visible" r:id="rId15"/>
-    <sheet name="Indicators" sheetId="15" state="visible" r:id="rId16"/>
-    <sheet name="Volumes" sheetId="16" state="visible" r:id="rId17"/>
-    <sheet name="Matrices" sheetId="17" state="visible" r:id="rId18"/>
-    <sheet name="Pairings" sheetId="18" state="visible" r:id="rId19"/>
+    <sheet name="Trajectories" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="Reducers" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="Indicators" sheetId="16" state="visible" r:id="rId17"/>
+    <sheet name="Volumes" sheetId="17" state="visible" r:id="rId18"/>
+    <sheet name="Matrices" sheetId="18" state="visible" r:id="rId19"/>
+    <sheet name="Pairings" sheetId="19" state="visible" r:id="rId20"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="132">
   <si>
     <t xml:space="preserve">Sound Scape Explorer</t>
   </si>
@@ -70,35 +71,8 @@
     <t xml:space="preserve">audio_host</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">The host name serving your audio files.
-For Docker, use '</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">http://localhost:5531</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">'.</t>
-    </r>
+    <t xml:space="preserve">The host name serving your audio files.
+For Docker, use `http://localhost:5531`.</t>
   </si>
   <si>
     <t xml:space="preserve">expected_sample_rate</t>
@@ -267,7 +241,7 @@
     <t xml:space="preserve">date</t>
   </si>
   <si>
-    <t xml:space="preserve">The file date. Format `YYYYMMDD HHMM`.</t>
+    <t xml:space="preserve">The file date (ISO 8601 format).</t>
   </si>
   <si>
     <t xml:space="preserve">site</t>
@@ -330,44 +304,60 @@
     <t xml:space="preserve">start</t>
   </si>
   <si>
-    <t xml:space="preserve">The start date. Format `YYYYMMDD HHMM`.</t>
+    <t xml:space="preserve">The start date (ISO 8601 format).</t>
   </si>
   <si>
     <t xml:space="preserve">end</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The end date. Format `YYYYMMDD HHMM`.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reducers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reducer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The reducer. See `HelpReducers` tab for available options.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dimensions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of dimensions to reduce to.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bands</t>
   </si>
   <si>
     <r>
       <rPr>
-        <b val="true"/>
-        <i val="true"/>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Optional</t>
+      <t xml:space="preserve">The end date (</t>
     </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ISO 8601 format).</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Autoclusters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">autocluster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The autoclustering algorithm.
+See `HelpAutoclusters` tab for available options.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reducers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reducer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The reducing algorithm.
+See `HelpReducers` tab for available options.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dimensions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of dimensions to reduce to.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bands</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <i val="true"/>
@@ -376,13 +366,10 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> The list of band names to consider. Separate with `,`. If empty, all bands will be processed.</t>
+      <t xml:space="preserve">The list of band names to consider.
+Separate with `,`. If empty, all bands will be processed.
+</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">integrations</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b val="true"/>
@@ -390,10 +377,23 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Optional</t>
+      <t xml:space="preserve">Optional, Default</t>
     </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> all bands</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">integrations</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <i val="true"/>
@@ -402,13 +402,10 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> The list of integration names to consider. Separate with `,`. If empty, all integrations will be processed.</t>
+      <t xml:space="preserve">The list of integration names to consider.
+Separate with `,`. If empty, all integrations will be processed.
+</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">ranges</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b val="true"/>
@@ -416,10 +413,23 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Optional</t>
+      <t xml:space="preserve">Optional, Default</t>
     </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> all integrations</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ranges</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <i val="true"/>
@@ -428,8 +438,38 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> The list of range names to consider. Separate with `,`. If empty, all ranges will be processed.</t>
+      <t xml:space="preserve">The list of range names to consider.
+Separate with `,`. If empty, all ranges will be processed.
+</t>
     </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Optional, Default</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> all ranges</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Trajectories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trajectory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The trajectory name.</t>
   </si>
   <si>
     <t xml:space="preserve">Indicators</t>
@@ -438,7 +478,8 @@
     <t xml:space="preserve">indicator</t>
   </si>
   <si>
-    <t xml:space="preserve">The indicator. See `HelpIndicators` tab for available options.</t>
+    <t xml:space="preserve">The indicator.
+See `HelpIndicators` tab for available options.</t>
   </si>
   <si>
     <t xml:space="preserve">Volumes</t>
@@ -447,7 +488,8 @@
     <t xml:space="preserve">volume</t>
   </si>
   <si>
-    <t xml:space="preserve">The indicator. See `HelpVolumes` tab for available options.</t>
+    <t xml:space="preserve">The volume.
+See `HelpVolumes` tab for available options.</t>
   </si>
   <si>
     <t xml:space="preserve">Matrices</t>
@@ -456,7 +498,8 @@
     <t xml:space="preserve">matrix</t>
   </si>
   <si>
-    <t xml:space="preserve">The matrix. See `HelpMatrices` tab for available options.</t>
+    <t xml:space="preserve">The matrix.
+See `HelpMatrices` tab for available options.</t>
   </si>
   <si>
     <t xml:space="preserve">Pairings</t>
@@ -465,10 +508,8 @@
     <t xml:space="preserve">pairing</t>
   </si>
   <si>
-    <t xml:space="preserve">The pairing. See `HelpPairings` tab for available options.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">autocluster</t>
+    <t xml:space="preserve">The pairing.
+See `HelpPairings` tab for available options.</t>
   </si>
   <si>
     <t xml:space="preserve">hdbscan-eom</t>
@@ -628,6 +669,9 @@
   </si>
   <si>
     <t xml:space="preserve">epsilon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">my_day_trajectory</t>
   </si>
 </sst>
 </file>
@@ -639,7 +683,7 @@
     <numFmt numFmtId="165" formatCode="General"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -685,13 +729,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b val="true"/>
       <i val="true"/>
       <sz val="10"/>
@@ -702,6 +739,31 @@
     <font>
       <i val="true"/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <i val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -801,7 +863,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="35">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -834,31 +896,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -874,8 +924,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -890,15 +944,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -942,11 +996,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1028,12 +1082,12 @@
     <tabColor rgb="FFEEEEEE"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:B60"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B25" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
+      <selection pane="topRight" activeCell="A39" activeCellId="0" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1077,7 +1131,7 @@
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
         <v>7</v>
       </c>
@@ -1085,7 +1139,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
         <v>9</v>
       </c>
@@ -1094,42 +1148,42 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10" t="s">
+    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="s">
+    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="s">
+    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10" t="s">
+    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1140,7 +1194,7 @@
       <c r="B15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B16" s="7" t="s">
@@ -1148,7 +1202,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B17" s="7" t="s">
@@ -1156,7 +1210,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B18" s="7" t="s">
@@ -1164,7 +1218,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B19" s="7" t="s">
@@ -1178,7 +1232,7 @@
       <c r="B21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B22" s="7" t="s">
@@ -1186,7 +1240,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B23" s="7" t="s">
@@ -1194,7 +1248,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B24" s="7" t="s">
@@ -1208,7 +1262,7 @@
       <c r="B26" s="2"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="6" t="s">
         <v>38</v>
       </c>
       <c r="B27" s="7" t="s">
@@ -1216,7 +1270,7 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="6" t="s">
         <v>40</v>
       </c>
       <c r="B28" s="7" t="s">
@@ -1230,7 +1284,7 @@
       <c r="B30" s="2"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="6" t="s">
         <v>43</v>
       </c>
       <c r="B31" s="7" t="s">
@@ -1238,7 +1292,7 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="8" t="s">
+      <c r="A32" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B32" s="7" t="s">
@@ -1246,7 +1300,7 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="8" t="s">
+      <c r="A33" s="6" t="s">
         <v>47</v>
       </c>
       <c r="B33" s="7" t="s">
@@ -1259,57 +1313,57 @@
       </c>
       <c r="B35" s="2"/>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="8" t="s">
+    <row r="36" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="6" t="s">
         <v>50</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="8" t="s">
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B38" s="2"/>
+    </row>
+    <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="6" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="12" t="s">
+      <c r="B39" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B38" s="13" t="s">
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="6" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="12" t="s">
+      <c r="B40" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B39" s="13" t="s">
+    </row>
+    <row r="41" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="9" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="12" t="s">
+      <c r="B41" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B40" s="13" t="s">
+    </row>
+    <row r="42" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="9" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="2" t="s">
+      <c r="B42" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B42" s="2"/>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="8" t="s">
+    </row>
+    <row r="43" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B43" s="14" t="s">
+      <c r="B43" s="10" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1320,39 +1374,83 @@
       <c r="B45" s="2"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="8" t="s">
+      <c r="A46" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B46" s="14" t="s">
+      <c r="B46" s="11" t="s">
         <v>65</v>
       </c>
     </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B48" s="2"/>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="8" t="s">
+      <c r="B50" s="2"/>
+    </row>
+    <row r="51" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="B49" s="14" t="s">
+      <c r="B51" s="7" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="2" t="s">
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B51" s="2"/>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="8" t="s">
+      <c r="B53" s="2"/>
+    </row>
+    <row r="54" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B52" s="14" t="s">
+      <c r="B54" s="7" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B56" s="2"/>
+    </row>
+    <row r="57" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B59" s="2"/>
+    </row>
+    <row r="60" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1361,7 +1459,6 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" location="readme" display="Find documentation here: https://github.com/sound-scape-explorer/sound-scape-explorer#readme"/>
-    <hyperlink ref="B8" r:id="rId2" display="http://localhost:5531"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1381,7 +1478,7 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -1391,44 +1488,44 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="32" width="11.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="33" width="11.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="11.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="31" width="11.84"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="4" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="28" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="32" t="s">
-        <v>119</v>
-      </c>
-      <c r="B2" s="33" t="n">
+      <c r="A2" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" s="31" t="n">
         <v>20</v>
       </c>
-      <c r="C2" s="33" t="n">
+      <c r="C2" s="31" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1449,7 +1546,7 @@
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -1459,35 +1556,35 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="32" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="33" width="18.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="31" width="18.97"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1016" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="28" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="32" t="s">
-        <v>120</v>
-      </c>
-      <c r="B2" s="33" t="n">
+      <c r="A2" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" s="31" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="28"/>
+      <c r="B4" s="26"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="28"/>
+      <c r="B5" s="26"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="28"/>
+      <c r="B6" s="26"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1508,49 +1605,49 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="32" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="33" width="20.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="31" width="20.03"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="4" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="28" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="32" t="s">
-        <v>121</v>
-      </c>
-      <c r="B2" s="34" t="n">
+      <c r="A2" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" s="32" t="n">
         <v>44927</v>
       </c>
-      <c r="C2" s="34" t="n">
+      <c r="C2" s="32" t="n">
         <v>45292</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="28"/>
+      <c r="C4" s="26"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1571,7 +1668,7 @@
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -1581,46 +1678,46 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="32" width="16.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="33" width="16.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="28" width="17.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="28" width="15.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="28" width="25.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="16.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="31" width="16.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="26" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="26" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="26" width="25.98"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="6" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="B1" s="30" t="s">
-        <v>122</v>
-      </c>
-      <c r="C1" s="30" t="s">
-        <v>123</v>
-      </c>
-      <c r="D1" s="30" t="s">
-        <v>124</v>
-      </c>
-      <c r="E1" s="30" t="s">
-        <v>125</v>
+      <c r="A1" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>130</v>
       </c>
       <c r="F1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="B2" s="28" t="n">
+      <c r="A2" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="26" t="n">
         <v>15</v>
       </c>
-      <c r="C2" s="28" t="n">
+      <c r="C2" s="26" t="n">
         <v>15</v>
       </c>
-      <c r="D2" s="28" t="n">
+      <c r="D2" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="28" t="n">
+      <c r="E2" s="26" t="n">
         <v>0.1</v>
       </c>
     </row>
@@ -1651,59 +1748,117 @@
     <tabColor rgb="FFFFFFD7"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="32" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="33" width="14.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="33" width="17.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="33" width="15.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="33" width="25.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="31" width="18.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="31" width="21.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="26" width="21.26"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="4" style="1" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="B2" s="32" t="n">
+        <v>44958</v>
+      </c>
+      <c r="C2" s="32" t="n">
+        <v>44959</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <tabColor rgb="FFFFFFD7"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="31" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="31" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="31" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="31" width="25.98"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="6" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="B1" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" s="35" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" s="35" t="s">
-        <v>58</v>
+      <c r="A1" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>61</v>
       </c>
       <c r="F1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="B2" s="28" t="n">
+      <c r="A2" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="26" t="n">
         <v>3</v>
       </c>
-      <c r="C2" s="36" t="s">
-        <v>119</v>
-      </c>
-      <c r="D2" s="36" t="s">
-        <v>120</v>
-      </c>
-      <c r="E2" s="36" t="s">
-        <v>121</v>
+      <c r="C2" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1727,7 +1882,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFD7"/>
@@ -1735,7 +1890,7 @@
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -1745,18 +1900,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="32" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="13.17"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="30" t="s">
-        <v>61</v>
+      <c r="A1" s="28" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="32" t="s">
-        <v>96</v>
+      <c r="A2" s="30" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1780,7 +1935,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFD7"/>
@@ -1788,7 +1943,7 @@
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -1798,18 +1953,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="32" width="15.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="15.63"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="30" t="s">
-        <v>64</v>
+      <c r="A1" s="28" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="32" t="s">
-        <v>98</v>
+      <c r="A2" s="30" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1833,7 +1988,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFD7"/>
@@ -1841,7 +1996,7 @@
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -1851,18 +2006,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="32" width="15.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="15.63"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="30" t="s">
-        <v>67</v>
+      <c r="A1" s="28" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="32" t="s">
-        <v>110</v>
+      <c r="A2" s="30" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1882,7 +2037,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFD7"/>
@@ -1890,7 +2045,7 @@
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -1900,18 +2055,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="32" width="15.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="15.63"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="30" t="s">
-        <v>70</v>
+      <c r="A1" s="28" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="32" t="s">
-        <v>112</v>
+      <c r="A2" s="30" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1939,7 +2094,7 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -1949,23 +2104,23 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="15" width="16.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="16.24"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16" t="s">
-        <v>72</v>
+      <c r="A1" s="13" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="15" t="s">
-        <v>73</v>
+      <c r="A2" s="12" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="15" t="s">
-        <v>74</v>
+      <c r="A3" s="12" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1987,7 +2142,7 @@
   </sheetPr>
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -1997,33 +2152,33 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="15" width="16.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="16.24"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16" t="s">
-        <v>50</v>
+      <c r="A1" s="13" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="15" t="s">
-        <v>75</v>
+      <c r="A2" s="12" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="15" t="s">
-        <v>76</v>
+      <c r="A3" s="12" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="15" t="s">
-        <v>77</v>
+      <c r="A4" s="12" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="15" t="s">
-        <v>78</v>
+      <c r="A5" s="12" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -2045,7 +2200,7 @@
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -2055,89 +2210,89 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="15" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="42.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16" t="s">
-        <v>61</v>
+      <c r="A1" s="13" t="s">
+        <v>67</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>81</v>
+      <c r="A2" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>83</v>
+      <c r="A3" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>85</v>
+      <c r="A4" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>87</v>
+      <c r="A5" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>89</v>
+      <c r="A6" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>91</v>
+      <c r="A7" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>93</v>
+      <c r="A8" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>95</v>
+      <c r="A9" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>97</v>
+      <c r="A10" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -2159,7 +2314,7 @@
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -2169,65 +2324,65 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="15" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="42.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16" t="s">
-        <v>64</v>
+      <c r="A1" s="13" t="s">
+        <v>70</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>99</v>
+      <c r="A2" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>101</v>
+      <c r="A3" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>103</v>
+      <c r="A4" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>105</v>
+      <c r="A5" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="18"/>
+      <c r="B6" s="15"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="14"/>
+      <c r="B7" s="16"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="14"/>
+      <c r="B8" s="16"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="14"/>
+      <c r="B9" s="16"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="14"/>
+      <c r="B10" s="16"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2248,7 +2403,7 @@
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -2258,60 +2413,60 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="15" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="42.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16" t="s">
-        <v>67</v>
+      <c r="A1" s="13" t="s">
+        <v>73</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>107</v>
+      <c r="A2" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>109</v>
+      <c r="A3" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>111</v>
+      <c r="A4" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="18"/>
+      <c r="B5" s="15"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="18"/>
+      <c r="B6" s="15"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="14"/>
+      <c r="B7" s="16"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="14"/>
+      <c r="B8" s="16"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="14"/>
+      <c r="B9" s="16"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="14"/>
+      <c r="B10" s="16"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2332,7 +2487,7 @@
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -2342,50 +2497,50 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="15" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="42.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16" t="s">
-        <v>67</v>
+      <c r="A1" s="13" t="s">
+        <v>73</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>113</v>
+      <c r="A2" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="18"/>
+      <c r="B3" s="15"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="18"/>
+      <c r="B4" s="15"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="18"/>
+      <c r="B5" s="15"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="18"/>
+      <c r="B6" s="15"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="14"/>
+      <c r="B7" s="16"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="14"/>
+      <c r="B8" s="16"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="14"/>
+      <c r="B9" s="16"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="14"/>
+      <c r="B10" s="16"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2406,7 +2561,7 @@
   </sheetPr>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -2422,65 +2577,65 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>115</v>
+      <c r="A1" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="21" t="str">
+      <c r="B2" s="19" t="str">
         <f aca="false">"/path/to/your/audio/folder"</f>
         <v>/path/to/your/audio/folder</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="22" t="s">
-        <v>116</v>
+      <c r="B3" s="20" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="21" t="n">
+      <c r="B4" s="19" t="n">
         <v>44100</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="24"/>
+      <c r="B5" s="22"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="24" t="n">
+      <c r="B6" s="22" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="24" t="n">
+      <c r="B7" s="22" t="n">
         <v>50</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="24" t="n">
+      <c r="B8" s="22" t="n">
         <v>42000</v>
       </c>
     </row>
@@ -2506,7 +2661,7 @@
   </sheetPr>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -2516,71 +2671,71 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="25" width="56.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="26" width="42.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="27" width="22.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="4" style="28" width="20.56"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="34" min="11" style="29" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="56.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="24" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="25" width="22.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="4" style="26" width="20.56"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="34" min="11" style="27" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1009" min="35" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
+      <c r="D1" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="20" t="str">
+      <c r="A2" s="18" t="str">
         <f aca="false">"/path/from/audio/folder"</f>
         <v>/path/from/audio/folder</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="31" t="n">
+      <c r="C2" s="29" t="n">
         <v>45089.8854166667</v>
       </c>
-      <c r="D2" s="28" t="s">
-        <v>118</v>
+      <c r="D2" s="26" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="20"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="31"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="29"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="20"/>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="20"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="20"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="21"/>
+      <c r="C7" s="19"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
feat(Processing): Add `timeline` strategy grouping
Instead of iterating over files, the reference is now a starting
timestamp.

The application then adds integration duration increments and look up in
all files if there is any audio inside the given interval.

If data is found, audio features are fetched and averaged.

Please note that multiple audio files can overlap within a single
interval.

User has now to look up for `site` as the file reference.

In non simultaneous campaigns, this will not be a problem.

Looking for `Front` module adaptations in order to reflect these
changes.

BREAKING CHANGE: Excel configuration storage has now a new setting
`grouping_start`. Also, the nature of `Groups` / `Aggregates`
/ `Integrated` features have been changed due to `timeline` strategy
implementation.
</commit_message>
<xml_diff>
--- a/examples/common/config.xlsx
+++ b/examples/common/config.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="134">
   <si>
     <t xml:space="preserve">Sound Scape Explorer</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t xml:space="preserve">The sample rate of your audio samples in Hertz.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grouping_start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The date to start integration from.</t>
   </si>
   <si>
     <t xml:space="preserve">timezone</t>
@@ -310,23 +316,7 @@
     <t xml:space="preserve">end</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">The end date (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">ISO 8601 format).</t>
-    </r>
+    <t xml:space="preserve">The end date (ISO 8601 format).</t>
   </si>
   <si>
     <t xml:space="preserve">Autoclusters</t>
@@ -377,6 +367,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Optional, Default</t>
     </r>
@@ -386,6 +377,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> all bands</t>
     </r>
@@ -413,6 +405,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Optional, Default</t>
     </r>
@@ -422,6 +415,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> all integrations</t>
     </r>
@@ -449,6 +443,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Optional, Default</t>
     </r>
@@ -458,6 +453,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> all ranges</t>
     </r>
@@ -683,7 +679,7 @@
     <numFmt numFmtId="165" formatCode="General"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -742,24 +738,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <i val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -944,7 +922,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -980,10 +962,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -996,7 +974,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1082,12 +1060,12 @@
     <tabColor rgb="FFEEEEEE"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B60"/>
+  <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B25" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
-      <selection pane="topRight" activeCell="A39" activeCellId="0" sqref="A39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1155,11 +1133,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9" t="s">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="8" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1187,19 +1165,19 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
+    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B14" s="10" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="7" t="s">
+      <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="B16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
@@ -1225,19 +1203,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="s">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="2"/>
+      <c r="B20" s="7" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="7" t="s">
+      <c r="A22" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="B22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
@@ -1255,19 +1233,19 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2" t="s">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="2"/>
+      <c r="B25" s="7" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B27" s="7" t="s">
+      <c r="A27" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="B27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
@@ -1277,19 +1255,19 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2" t="s">
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="2"/>
+      <c r="B29" s="7" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B31" s="7" t="s">
+      <c r="A31" s="2" t="s">
         <v>44</v>
       </c>
+      <c r="B31" s="2"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="s">
@@ -1307,35 +1285,35 @@
         <v>48</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="2" t="s">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B35" s="2"/>
-    </row>
-    <row r="36" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="6" t="s">
+      <c r="B34" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B36" s="7" t="s">
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="2" t="s">
+      <c r="B36" s="2"/>
+    </row>
+    <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B38" s="2"/>
-    </row>
-    <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="6" t="s">
+      <c r="B37" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B39" s="7" t="s">
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="2"/>
+    </row>
+    <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="6" t="s">
         <v>55</v>
       </c>
@@ -1343,11 +1321,11 @@
         <v>56</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="9" t="s">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B41" s="10" t="s">
+      <c r="B41" s="7" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1367,26 +1345,26 @@
         <v>62</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="2" t="s">
+    <row r="44" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B45" s="2"/>
+      <c r="B44" s="10" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B46" s="11" t="s">
+      <c r="A46" s="2" t="s">
         <v>65</v>
       </c>
+      <c r="B46" s="2"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B47" s="7" t="s">
-        <v>46</v>
+        <v>66</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1397,60 +1375,68 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B50" s="2"/>
-    </row>
-    <row r="51" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B51" s="7" t="s">
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="2" t="s">
+      <c r="B51" s="2"/>
+    </row>
+    <row r="52" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B53" s="2"/>
-    </row>
-    <row r="54" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="6" t="s">
+      <c r="B52" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B54" s="7" t="s">
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="2" t="s">
+      <c r="B54" s="2"/>
+    </row>
+    <row r="55" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B56" s="2"/>
-    </row>
-    <row r="57" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="6" t="s">
+      <c r="B55" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B57" s="7" t="s">
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="2" t="s">
+      <c r="B57" s="2"/>
+    </row>
+    <row r="58" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B59" s="2"/>
-    </row>
-    <row r="60" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="6" t="s">
+      <c r="B58" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B60" s="7" t="s">
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="2" t="s">
         <v>77</v>
+      </c>
+      <c r="B60" s="2"/>
+    </row>
+    <row r="61" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1494,19 +1480,19 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="B1" s="29" t="s">
         <v>35</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="30" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B2" s="31" t="n">
         <v>20</v>
@@ -1516,16 +1502,16 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1562,29 +1548,29 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>40</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="30" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B2" s="31" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="26"/>
+      <c r="B4" s="27"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="26"/>
+      <c r="B5" s="27"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="26"/>
+      <c r="B6" s="27"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1621,19 +1607,19 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="B1" s="29" t="s">
         <v>47</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="30" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B2" s="32" t="n">
         <v>44927</v>
@@ -1643,11 +1629,11 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="26"/>
+      <c r="C4" s="27"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1680,44 +1666,44 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="16.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="31" width="16.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="26" width="17.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="26" width="15.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="26" width="25.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="27" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="27" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="27" width="25.98"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="6" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="B1" s="28" t="s">
-        <v>127</v>
-      </c>
-      <c r="C1" s="28" t="s">
-        <v>128</v>
-      </c>
-      <c r="D1" s="28" t="s">
+      <c r="A1" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="C1" s="29" t="s">
         <v>130</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>132</v>
       </c>
       <c r="F1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="30" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2" s="26" t="n">
+        <v>80</v>
+      </c>
+      <c r="B2" s="27" t="n">
         <v>15</v>
       </c>
-      <c r="C2" s="26" t="n">
+      <c r="C2" s="27" t="n">
         <v>15</v>
       </c>
-      <c r="D2" s="26" t="n">
+      <c r="D2" s="27" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="26" t="n">
+      <c r="E2" s="27" t="n">
         <v>0.1</v>
       </c>
     </row>
@@ -1762,25 +1748,25 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="31" width="18.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="31" width="21.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="26" width="21.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="27" width="21.26"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="4" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="B1" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" s="28" t="s">
+      <c r="A1" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="29" t="s">
         <v>47</v>
       </c>
+      <c r="C1" s="29" t="s">
+        <v>49</v>
+      </c>
       <c r="D1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
-        <v>131</v>
+      <c r="A2" s="27" t="s">
+        <v>133</v>
       </c>
       <c r="B2" s="32" t="n">
         <v>44958</v>
@@ -1827,38 +1813,38 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>55</v>
       </c>
+      <c r="B1" s="29" t="s">
+        <v>57</v>
+      </c>
       <c r="C1" s="33" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D1" s="33" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E1" s="33" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="B2" s="26" t="n">
+        <v>82</v>
+      </c>
+      <c r="B2" s="27" t="n">
         <v>3</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1905,13 +1891,13 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28" t="s">
-        <v>67</v>
+      <c r="A1" s="29" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="30" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1958,13 +1944,13 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28" t="s">
-        <v>70</v>
+      <c r="A1" s="29" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="30" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -2011,13 +1997,13 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28" t="s">
-        <v>73</v>
+      <c r="A1" s="29" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="30" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -2060,13 +2046,13 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28" t="s">
-        <v>76</v>
+      <c r="A1" s="29" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="30" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -2110,17 +2096,17 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2158,27 +2144,27 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="12" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="12" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2217,82 +2203,82 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="12" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="12" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="12" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="12" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -2331,42 +2317,42 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="12" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="12" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2420,34 +2406,34 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="12" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2504,18 +2490,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2559,14 +2545,14 @@
     <tabColor rgb="FFFFFFD7"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2578,10 +2564,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2598,7 +2584,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2610,32 +2596,40 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="22"/>
+      <c r="B5" s="21" t="n">
+        <v>45089.8854166667</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="22" t="n">
+      <c r="B6" s="23"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="23" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="22" t="n">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="23" t="n">
         <v>50</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="22" t="n">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="23" t="n">
         <v>42000</v>
       </c>
     </row>
@@ -2666,38 +2660,38 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="56.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="24" width="42.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="25" width="22.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="4" style="26" width="20.56"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="34" min="11" style="27" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="24" width="56.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="26" width="22.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="4" style="27" width="20.56"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="34" min="11" style="28" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1009" min="35" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B1" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="28" t="s">
-        <v>122</v>
-      </c>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="D1" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="18" t="str">
@@ -2705,19 +2699,19 @@
         <v>/path/from/audio/folder</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="29" t="n">
+        <v>28</v>
+      </c>
+      <c r="C2" s="21" t="n">
         <v>45089.8854166667</v>
       </c>
-      <c r="D2" s="26" t="s">
-        <v>123</v>
+      <c r="D2" s="27" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="18"/>
       <c r="B3" s="19"/>
-      <c r="C3" s="29"/>
+      <c r="C3" s="21"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="18"/>

</xml_diff>

<commit_message>
feat(Examples): Update template configuration file
</commit_message>
<xml_diff>
--- a/examples/common/config.xlsx
+++ b/examples/common/config.xlsx
@@ -9,24 +9,21 @@
   </bookViews>
   <sheets>
     <sheet name="Help" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="HelpAutoclusters" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="HelpReducers" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="HelpIndicators" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="HelpVolumes" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="HelpMatrices" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="HelpPairings" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="Settings" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="Files" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="Bands" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="Integrations" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="Ranges" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="Autoclusters" sheetId="13" state="visible" r:id="rId14"/>
-    <sheet name="Trajectories" sheetId="14" state="visible" r:id="rId15"/>
-    <sheet name="Reducers" sheetId="15" state="visible" r:id="rId16"/>
-    <sheet name="Indicators" sheetId="16" state="visible" r:id="rId17"/>
-    <sheet name="Volumes" sheetId="17" state="visible" r:id="rId18"/>
-    <sheet name="Matrices" sheetId="18" state="visible" r:id="rId19"/>
-    <sheet name="Pairings" sheetId="19" state="visible" r:id="rId20"/>
+    <sheet name="ListExtractors" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="ListDigesters" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="ListReducers" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="ListAutoclusters" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="ListTrajectories" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Settings" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Files" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Bands" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Integrations" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Ranges" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="Extractors" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="Digesters" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="Reducers" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="Autoclusters" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="Trajectories" sheetId="16" state="visible" r:id="rId17"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -37,8 +34,67 @@
 </workbook>
 </file>
 
+<file path=xl/comments12.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">milliseconds</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">milliseconds</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments14.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Use 2 or 3 unless not human</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="144">
   <si>
     <t xml:space="preserve">Sound Scape Explorer</t>
   </si>
@@ -81,7 +137,7 @@
     <t xml:space="preserve">The sample rate of your audio samples in Hertz.</t>
   </si>
   <si>
-    <t xml:space="preserve">grouping_start</t>
+    <t xml:space="preserve">timeline_origin</t>
   </si>
   <si>
     <t xml:space="preserve">The date to start integration from.</t>
@@ -256,10 +312,10 @@
     <t xml:space="preserve">The site.</t>
   </si>
   <si>
-    <t xml:space="preserve">meta_X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The meta properties. Rename `X` and add your metas.</t>
+    <t xml:space="preserve">label_PROPERTY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The label properties. Rename PROPERTY accordingly and add your label values.</t>
   </si>
   <si>
     <t xml:space="preserve">Bands</t>
@@ -319,14 +375,58 @@
     <t xml:space="preserve">The end date (ISO 8601 format).</t>
   </si>
   <si>
+    <t xml:space="preserve">Extractors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extractor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The extractor name.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">offset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The offset for each file in milliseconds.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">step</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The step to iterate in milliseconds.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">persist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whether the extracted data should be stored.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digesters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">digester</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The digester name.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Autoclusters</t>
   </si>
   <si>
     <t xml:space="preserve">autocluster</t>
   </si>
   <si>
-    <t xml:space="preserve">The autoclustering algorithm.
-See `HelpAutoclusters` tab for available options.</t>
+    <t xml:space="preserve">The autoclustering algorithm.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trajectories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trajectory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The trajectory name.</t>
   </si>
   <si>
     <t xml:space="preserve">Reducers</t>
@@ -335,7 +435,7 @@
     <t xml:space="preserve">reducer</t>
   </si>
   <si>
-    <t xml:space="preserve">The reducing algorithm.
+    <t xml:space="preserve">The reducer name.
 See `HelpReducers` tab for available options.</t>
   </si>
   <si>
@@ -459,53 +559,127 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Trajectories</t>
-  </si>
-  <si>
-    <t xml:space="preserve">trajectory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The trajectory name.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indicators</t>
-  </si>
-  <si>
     <t xml:space="preserve">indicator</t>
   </si>
   <si>
-    <t xml:space="preserve">The indicator.
-See `HelpIndicators` tab for available options.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volumes</t>
+    <t xml:space="preserve">description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vgg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The VGGish neural network.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">leq_maad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Leq using maad library.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">med</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The temporal median.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ht</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The temporal entropy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The frequency entropy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aci</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The acoustic complexity index.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The acoustic diversity index.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The bioacoustics index.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ndsi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The normalized difference soundscape index.</t>
   </si>
   <si>
     <t xml:space="preserve">volume</t>
   </si>
   <si>
-    <t xml:space="preserve">The volume.
-See `HelpVolumes` tab for available options.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Matrices</t>
-  </si>
-  <si>
-    <t xml:space="preserve">matrix</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The matrix.
-See `HelpMatrices` tab for available options.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pairings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pairing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The pairing.
-See `HelpPairings` tab for available options.</t>
+    <t xml:space="preserve">sum_var</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The sum variance.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sum_std</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The sum standard deviation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mean_std</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The mean standard deviation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mean_spreading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The mean spreading.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">distance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The distance between subtypes of a given cluster.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">overlap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The overlap between subtypes of a given cluster.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">silhouette</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The silhouette between subtypes of a given cluster.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contingency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contingency between two clusters.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">umap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sparse_pca</t>
   </si>
   <si>
     <t xml:space="preserve">hdbscan-eom</t>
@@ -514,121 +688,13 @@
     <t xml:space="preserve">hdbscan-leaf</t>
   </si>
   <si>
-    <t xml:space="preserve">umap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vae</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sparse_pca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">leq_enes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Leq with ENES’ method.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">leq_maad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Leq using maad library.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">med</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The temporal median.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ht</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The temporal entropy.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The frequency entropy.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aci</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The acoustic complexity index.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">adi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The acoustic diversity index.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The bioacoustics index.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ndsi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The normalized difference soundscape index.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sum_var</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The sum variance.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sum_std</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The sum standard deviation.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mean_std</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The mean standard deviation.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mean_spreading</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The mean spreading.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">distance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The distance between subtypes of a given cluster.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">overlap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The overlap between subtypes of a given cluster.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">silhouette</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The silhouette between subtypes of a given cluster.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contingency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contingency between two clusters.</t>
+    <t xml:space="preserve">hour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">month</t>
   </si>
   <si>
     <t xml:space="preserve">setting</t>
@@ -640,12 +706,6 @@
     <t xml:space="preserve">http://localhost:5531</t>
   </si>
   <si>
-    <t xml:space="preserve">meta_LABEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">label</t>
-  </si>
-  <si>
     <t xml:space="preserve">human</t>
   </si>
   <si>
@@ -655,6 +715,9 @@
     <t xml:space="preserve">r2023</t>
   </si>
   <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
     <t xml:space="preserve">min_cluster_size</t>
   </si>
   <si>
@@ -667,7 +730,25 @@
     <t xml:space="preserve">epsilon</t>
   </si>
   <si>
-    <t xml:space="preserve">my_day_trajectory</t>
+    <t xml:space="preserve">label_property</t>
+  </si>
+  <si>
+    <t xml:space="preserve">label_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">day1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIEU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">naturel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">day2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">day3</t>
   </si>
 </sst>
 </file>
@@ -841,7 +922,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -886,6 +967,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -894,14 +979,14 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -979,6 +1064,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1060,12 +1153,12 @@
     <tabColor rgb="FFEEEEEE"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B61"/>
+  <dimension ref="A1:B58"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1204,10 +1297,10 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="12" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1299,7 +1392,7 @@
       </c>
       <c r="B36" s="2"/>
     </row>
-    <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="s">
         <v>52</v>
       </c>
@@ -1307,103 +1400,103 @@
         <v>53</v>
       </c>
     </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B39" s="2"/>
-    </row>
-    <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="6" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B42" s="10" t="s">
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="43" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="9" t="s">
+      <c r="B42" s="2"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="B43" s="7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="9" t="s">
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B44" s="10" t="s">
+      <c r="B45" s="2"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="6" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="2" t="s">
+      <c r="B46" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B46" s="2"/>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="6" t="s">
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B47" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>48</v>
-      </c>
+      <c r="B48" s="2"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B49" s="7" t="s">
+      <c r="B51" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B51" s="2"/>
-    </row>
-    <row r="52" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="6" t="s">
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="B53" s="2"/>
+    </row>
+    <row r="54" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="6" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="2" t="s">
+      <c r="B54" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B54" s="2"/>
-    </row>
-    <row r="55" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="6" t="s">
         <v>72</v>
       </c>
@@ -1411,31 +1504,27 @@
         <v>73</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="2" t="s">
+    <row r="56" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B57" s="2"/>
-    </row>
-    <row r="58" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="6" t="s">
+      <c r="B56" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="B58" s="7" t="s">
+    </row>
+    <row r="57" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="9" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="2" t="s">
+      <c r="B57" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="B60" s="2"/>
-    </row>
-    <row r="61" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="6" t="s">
+    </row>
+    <row r="58" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="B61" s="7" t="s">
+      <c r="B58" s="10" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1462,56 +1551,47 @@
     <tabColor rgb="FFFFFFD7"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="11.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="31" width="11.84"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="4" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="31" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="32" width="18.97"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1016" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="29" t="s">
-        <v>37</v>
+      <c r="A1" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30" t="s">
-        <v>126</v>
-      </c>
-      <c r="B2" s="31" t="n">
-        <v>20</v>
-      </c>
-      <c r="C2" s="31" t="n">
-        <v>20000</v>
+      <c r="A2" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" s="32" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
+      <c r="B4" s="28"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
+      <c r="B5" s="28"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
+      <c r="B6" s="28"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1530,7 +1610,7 @@
     <tabColor rgb="FFFFFFD7"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -1542,35 +1622,39 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="31" width="18.97"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1016" min="3" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="31" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="32" width="20.03"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="4" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="29" t="s">
-        <v>42</v>
+      <c r="A1" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="B2" s="31" t="n">
-        <v>15</v>
-      </c>
+      <c r="A2" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="B2" s="33" t="n">
+        <v>44927</v>
+      </c>
+      <c r="C2" s="33" t="n">
+        <v>45292</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="27"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="27"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="27"/>
+      <c r="C4" s="28"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1589,53 +1673,57 @@
     <tabColor rgb="FFFFFFD7"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="31" width="20.03"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="4" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="31" width="10.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="32" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="28" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="28" width="15.45"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1013" min="5" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="C1" s="29" t="s">
-        <v>49</v>
-      </c>
+      <c r="A1" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30" t="s">
-        <v>128</v>
+      <c r="A2" s="31" t="s">
+        <v>82</v>
       </c>
       <c r="B2" s="32" t="n">
-        <v>44927</v>
-      </c>
-      <c r="C2" s="32" t="n">
-        <v>45292</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="27"/>
+        <v>0</v>
+      </c>
+      <c r="C2" s="28" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>132</v>
+      </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1002" type="list">
+      <formula1>ListExtractors!$A$2:$A$1048576</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1643,6 +1731,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1652,69 +1741,56 @@
     <tabColor rgb="FFFFFFD7"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="16.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="31" width="16.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="27" width="17.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="27" width="15.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="27" width="25.98"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="6" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="31" width="15.63"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="29" t="s">
-        <v>129</v>
-      </c>
-      <c r="C1" s="29" t="s">
-        <v>130</v>
-      </c>
-      <c r="D1" s="29" t="s">
-        <v>131</v>
-      </c>
-      <c r="E1" s="29" t="s">
-        <v>132</v>
-      </c>
-      <c r="F1" s="0"/>
+      <c r="A1" s="30" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="B2" s="27" t="n">
-        <v>15</v>
-      </c>
-      <c r="C2" s="27" t="n">
-        <v>15</v>
-      </c>
-      <c r="D2" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" s="27" t="n">
-        <v>0.1</v>
+      <c r="A2" s="31" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="31" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="31" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="31" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="31" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1002" type="list">
-      <formula1>HelpAutoclusters!$A$2:$A$1048576</formula1>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1" type="none">
+      <formula1>Help!$A$2:$A$1048576</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1" type="none">
-      <formula1>HelpAutoclusters!$A$2:$A$1048576</formula1>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1006" type="list">
+      <formula1>ListDigesters!$A$2:$A$1048576</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -1734,48 +1810,70 @@
     <tabColor rgb="FFFFFFD7"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="31" width="18.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="31" width="21.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="27" width="21.26"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="4" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="31" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="32" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="32" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="32" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="32" width="25.98"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="6" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="B1" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="C1" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="D1" s="0"/>
+      <c r="A1" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="B2" s="32" t="n">
-        <v>44958</v>
-      </c>
-      <c r="C2" s="32" t="n">
-        <v>44959</v>
+      <c r="A2" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" s="32" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1" type="none">
+      <formula1>ListAutoclusters!$A$2:$A$1048576</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1003" type="list">
+      <formula1>ListReducers!$A$2:$A$1048576</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1783,6 +1881,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1799,62 +1898,62 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="31" width="14.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="31" width="17.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="31" width="15.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="31" width="25.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="31" width="16.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="32" width="16.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="28" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="28" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="28" width="25.98"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="6" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" s="33" t="s">
-        <v>63</v>
+      <c r="A1" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>136</v>
       </c>
       <c r="F1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="B2" s="27" t="n">
-        <v>3</v>
-      </c>
-      <c r="C2" s="34" t="s">
-        <v>126</v>
-      </c>
-      <c r="D2" s="34" t="s">
-        <v>127</v>
-      </c>
-      <c r="E2" s="34" t="s">
-        <v>128</v>
+      <c r="A2" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" s="28" t="n">
+        <v>15</v>
+      </c>
+      <c r="C2" s="28" t="n">
+        <v>15</v>
+      </c>
+      <c r="D2" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="28" t="n">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1002" type="list">
-      <formula1>HelpReducers!$A$2:$A$1048576</formula1>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1" type="none">
+      <formula1>ListAutoclusters!$A$2:$A$1048576</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1" type="none">
-      <formula1>HelpReducers!$A$2:$A$1048576</formula1>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1002" type="list">
+      <formula1>ListAutoclusters!$A$2:$A$1048576</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -1874,191 +1973,111 @@
     <tabColor rgb="FFFFFFD7"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="13.17"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="31" width="16.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="32" width="26.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="32" width="18.2"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="7" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="29" t="s">
-        <v>69</v>
+      <c r="A1" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30" t="s">
-        <v>103</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1002" type="list">
-      <formula1>HelpIndicators!$A$2:$A$1048576</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1" type="none">
-      <formula1>HelpIndicators!$A$2:$A$1048576</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <tabColor rgb="FFFFFFD7"/>
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="15.63"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="29" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30" t="s">
-        <v>105</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1002" type="list">
-      <formula1>HelpVolumes!$A$2:$A$1048576</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1" type="none">
-      <formula1>HelpVolumes!$A$2:$A$1048576</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <tabColor rgb="FFFFFFD7"/>
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="15.63"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="29" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30" t="s">
-        <v>117</v>
-      </c>
+      <c r="A2" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="B2" s="33" t="n">
+        <v>44881.5</v>
+      </c>
+      <c r="C2" s="33" t="n">
+        <v>44882.5416666667</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>140</v>
+      </c>
+      <c r="E2" s="33" t="s">
+        <v>141</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="31" t="s">
+        <v>142</v>
+      </c>
+      <c r="B3" s="33" t="n">
+        <v>44887.5</v>
+      </c>
+      <c r="C3" s="33" t="n">
+        <v>44888.5416666667</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>140</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>141</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" s="33" t="n">
+        <v>44907.5</v>
+      </c>
+      <c r="C4" s="33" t="n">
+        <v>44908.5416666667</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>140</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>141</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1:A1002" type="list">
-      <formula1>HelpMatrices!$A$2:$A$1048576</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <tabColor rgb="FFFFFFD7"/>
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="15.63"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="29" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30" t="s">
-        <v>119</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1:A1001" type="list">
-      <formula1>HelpPairings!$A$2:$A$1048576</formula1>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F2:F1004" type="list">
+      <formula1>ListTrajectories!$A$2:$A$1048576</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -2078,35 +2097,101 @@
     <tabColor rgb="FFEEEEEE"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="16.24"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="2" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="42.79"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
-        <v>52</v>
+      <c r="A1" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
-        <v>80</v>
+      <c r="A2" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="s">
-        <v>81</v>
+      <c r="A3" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -2126,46 +2211,97 @@
     <tabColor rgb="FFEEEEEE"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="16.24"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="2" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="42.79"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
-        <v>55</v>
+      <c r="A1" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
-        <v>82</v>
+      <c r="A2" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="s">
-        <v>83</v>
+      <c r="A3" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
-        <v>84</v>
+      <c r="A4" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12" t="s">
-        <v>85</v>
-      </c>
+      <c r="A5" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="17"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2184,7 +2320,7 @@
     <tabColor rgb="FFEEEEEE"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -2196,89 +2332,33 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="42.79"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="16.24"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>86</v>
+      <c r="A1" s="15" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>88</v>
+      <c r="A2" s="13" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>90</v>
+      <c r="A3" s="13" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>92</v>
+      <c r="A4" s="13" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>104</v>
+      <c r="A5" s="13" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2298,77 +2378,36 @@
     <tabColor rgb="FFEEEEEE"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="42.79"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="16.24"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>86</v>
+      <c r="A1" s="15" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>106</v>
+      <c r="A2" s="13" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="15"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="16"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="16"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="16"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="16"/>
+      <c r="A3" s="13" t="s">
+        <v>122</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2387,72 +2426,37 @@
     <tabColor rgb="FFEEEEEE"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="42.79"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="16.79"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>86</v>
+      <c r="A1" s="15" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>114</v>
+      <c r="A2" s="13" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>116</v>
+      <c r="A3" s="13" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="15"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="15"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="16"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="16"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="16"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="16"/>
+      <c r="A4" s="13" t="s">
+        <v>125</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2468,67 +2472,101 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
-    <tabColor rgb="FFEEEEEE"/>
+    <tabColor rgb="FFFFFFD7"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="42.79"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="29.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.24"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>86</v>
+      <c r="A1" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>120</v>
+      <c r="A2" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="20" t="str">
+        <f aca="false">"/path/to/your/audio/folder"</f>
+        <v>/path/to/your/audio/folder</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="15"/>
+      <c r="A3" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="15"/>
+      <c r="A4" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="20" t="n">
+        <v>44100</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="15"/>
+      <c r="A5" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="22" t="n">
+        <v>45089.8854166667</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="15"/>
+      <c r="A6" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="24"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="16"/>
+      <c r="A7" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="24" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="16"/>
+      <c r="A8" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="24" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="16"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="16"/>
+      <c r="A9" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="24" t="n">
+        <v>42000</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" display="http://localhost:5531"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2545,98 +2583,85 @@
     <tabColor rgb="FFFFFFD7"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="29.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.24"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="3" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="25" width="56.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="26" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="27" width="22.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="4" style="28" width="20.56"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="34" min="11" style="29" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1009" min="35" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>122</v>
-      </c>
+      <c r="A1" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="19" t="str">
-        <f aca="false">"/path/to/your/audio/folder"</f>
-        <v>/path/to/your/audio/folder</v>
+      <c r="A2" s="19" t="str">
+        <f aca="false">"/path/from/audio/folder"</f>
+        <v>/path/from/audio/folder</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="22" t="n">
+        <v>45089.8854166667</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>123</v>
-      </c>
+      <c r="A3" s="19"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="22"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="19" t="n">
-        <v>44100</v>
-      </c>
+      <c r="A4" s="19"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="21" t="n">
-        <v>45089.8854166667</v>
-      </c>
+      <c r="A5" s="19"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="23"/>
+      <c r="A6" s="19"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="23" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="23" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="23" t="n">
-        <v>42000</v>
-      </c>
+      <c r="C7" s="20"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="http://localhost:5531"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2653,83 +2678,56 @@
     <tabColor rgb="FFFFFFD7"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="24" width="56.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="42.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="26" width="22.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="4" style="27" width="20.56"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="34" min="11" style="28" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1009" min="35" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="31" width="11.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="32" width="11.84"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="4" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="29" t="s">
-        <v>124</v>
-      </c>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
+      <c r="A1" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="18" t="str">
-        <f aca="false">"/path/from/audio/folder"</f>
-        <v>/path/from/audio/folder</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="21" t="n">
-        <v>45089.8854166667</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="18"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="21"/>
+      <c r="A2" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="32" t="n">
+        <v>20</v>
+      </c>
+      <c r="C2" s="32" t="n">
+        <v>20000</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="18"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="18"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="18"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="19"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>